<commit_message>
Flow_Clackamas.xml - Add wetland reports. CW3MdigitalHandbook.docx - Add details to the McKenzie wetlands section.  Add a stub for a Clackamas basin section. Flow_McKenzie.xml - Revise and expand the wetland reports. CW3M_McKenzie_Script.iss - This is the version for the CW3M 0.3.3 release.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C84A808-DC35-4E0D-BB4A-48C4551056B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C011A88-37EB-4C3A-8114-BC0E25F513AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
@@ -557,7 +557,7 @@
       <pane xSplit="10" ySplit="13" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34:K35"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,8 +1630,16 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
+      <c r="B36" s="4">
+        <f>SUM(B38:B55)</f>
+        <v>519.25480000000005</v>
+      </c>
       <c r="D36" s="8" t="s">
         <v>37</v>
+      </c>
+      <c r="E36" s="4">
+        <f>SUM(E38:E49)</f>
+        <v>203.6249</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1879,8 +1887,8 @@
   <dimension ref="A1:K143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A144" sqref="A144:XFD144"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,6 +4018,10 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <f>SUM(B2:B102)</f>
+        <v>65</v>
+      </c>
       <c r="F103" s="5"/>
       <c r="G103" s="4"/>
     </row>

</xml_diff>

<commit_message>
Add InitWETL_CAPifNecessary() to facilitate turning on new wetlands in the wetland model. APs.cpp - Replace existing logic in RunPrescribedLULCs() with a call to InitWETL_CAPifNecessary(). Flow.h - Add "FLOWAPI" to the Wetland class declaration. Add InitWETL_CAPifNecessary(). Add a call to it in InitWetlands().
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A14E289-DEFC-4007-8BEE-44CBF25D02E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44314D75-7FFB-4C5D-953F-31CD12970DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
   <sheets>
     <sheet name="WETL_ID" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="50">
   <si>
     <t>WETL_ID</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t># of HRUs</t>
+  </si>
+  <si>
+    <t>Z_MIN, ft</t>
+  </si>
+  <si>
+    <t>Z_MIN, m</t>
+  </si>
+  <si>
+    <t>Z_MAX, ft</t>
+  </si>
+  <si>
+    <t>Z_MAX, m</t>
   </si>
 </sst>
 </file>
@@ -649,11 +661,11 @@
         <v>5</v>
       </c>
       <c r="H3" s="4">
-        <f>IDUs!H8</f>
+        <f>IDUs!L8</f>
         <v>24.105699999999999</v>
       </c>
       <c r="I3" s="2">
-        <f>IDUs!I8</f>
+        <f>IDUs!M8</f>
         <v>114.80779151818864</v>
       </c>
     </row>
@@ -680,11 +692,11 @@
         <v>2</v>
       </c>
       <c r="H4" s="4">
-        <f>IDUs!H12</f>
+        <f>IDUs!L12</f>
         <v>12.8376</v>
       </c>
       <c r="I4" s="2">
-        <f>IDUs!I12</f>
+        <f>IDUs!M12</f>
         <v>115.87905496354458</v>
       </c>
     </row>
@@ -711,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="4">
-        <f>IDUs!H18</f>
+        <f>IDUs!L18</f>
         <v>19.5397</v>
       </c>
       <c r="I5" s="2">
@@ -741,11 +753,11 @@
         <v>2</v>
       </c>
       <c r="H6" s="4">
-        <f>IDUs!H22</f>
+        <f>IDUs!L22</f>
         <v>14.686299999999999</v>
       </c>
       <c r="I6" s="2">
-        <f>IDUs!I22</f>
+        <f>IDUs!M22</f>
         <v>120.46777268610882</v>
       </c>
     </row>
@@ -772,11 +784,11 @@
         <v>3</v>
       </c>
       <c r="H7" s="4">
-        <f>IDUs!H27</f>
+        <f>IDUs!L27</f>
         <v>35.198799999999999</v>
       </c>
       <c r="I7" s="2">
-        <f>IDUs!I27</f>
+        <f>IDUs!M27</f>
         <v>124.10821118901781</v>
       </c>
     </row>
@@ -803,11 +815,11 @@
         <v>1</v>
       </c>
       <c r="H8" s="4">
-        <f>IDUs!H30</f>
+        <f>IDUs!L30</f>
         <v>14.101699999999999</v>
       </c>
       <c r="I8" s="2">
-        <f>IDUs!I30</f>
+        <f>IDUs!M30</f>
         <v>122.91</v>
       </c>
     </row>
@@ -834,11 +846,11 @@
         <v>5</v>
       </c>
       <c r="H9" s="4">
-        <f>IDUs!H37</f>
+        <f>IDUs!L37</f>
         <v>33.111600000000003</v>
       </c>
       <c r="I9" s="2">
-        <f>IDUs!I37</f>
+        <f>IDUs!M37</f>
         <v>125.35983235482429</v>
       </c>
     </row>
@@ -862,11 +874,11 @@
         <v>1</v>
       </c>
       <c r="H10" s="4">
-        <f>IDUs!H40</f>
+        <f>IDUs!L40</f>
         <v>10.452</v>
       </c>
       <c r="I10" s="2">
-        <f>IDUs!I40</f>
+        <f>IDUs!M40</f>
         <v>128.61000000000001</v>
       </c>
     </row>
@@ -893,11 +905,11 @@
         <v>3</v>
       </c>
       <c r="H11" s="4">
-        <f>IDUs!H45</f>
+        <f>IDUs!L45</f>
         <v>30.7943</v>
       </c>
       <c r="I11" s="2">
-        <f>IDUs!I45</f>
+        <f>IDUs!M45</f>
         <v>128.65973004744384</v>
       </c>
     </row>
@@ -924,11 +936,11 @@
         <v>2</v>
       </c>
       <c r="H12" s="4">
-        <f>IDUs!H49</f>
+        <f>IDUs!L49</f>
         <v>8.4712999999999994</v>
       </c>
       <c r="I12" s="2">
-        <f>IDUs!I49</f>
+        <f>IDUs!M49</f>
         <v>131.56476101660903</v>
       </c>
     </row>
@@ -955,7 +967,7 @@
         <v>6</v>
       </c>
       <c r="H13" s="4">
-        <f>IDUs!H57</f>
+        <f>IDUs!L57</f>
         <v>36.640300000000003</v>
       </c>
       <c r="I13" s="2">
@@ -985,11 +997,11 @@
         <v>5</v>
       </c>
       <c r="H14" s="4">
-        <f>IDUs!H64</f>
+        <f>IDUs!L64</f>
         <v>26.276800000000001</v>
       </c>
       <c r="I14" s="2">
-        <f>IDUs!I64</f>
+        <f>IDUs!M64</f>
         <v>134.27690288100209</v>
       </c>
     </row>
@@ -1016,11 +1028,11 @@
         <v>1</v>
       </c>
       <c r="H15" s="4">
-        <f>IDUs!H67</f>
+        <f>IDUs!L67</f>
         <v>6.5331999999999999</v>
       </c>
       <c r="I15" s="2">
-        <f>IDUs!I67</f>
+        <f>IDUs!M67</f>
         <v>134.74</v>
       </c>
     </row>
@@ -1047,11 +1059,11 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <f>IDUs!H70</f>
+        <f>IDUs!L70</f>
         <v>15.457800000000001</v>
       </c>
       <c r="I16" s="2">
-        <f>IDUs!I70</f>
+        <f>IDUs!M70</f>
         <v>139.35</v>
       </c>
     </row>
@@ -1078,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="H17" s="4">
-        <f>IDUs!H89</f>
+        <f>IDUs!L89</f>
         <v>161.80410000000001</v>
       </c>
       <c r="I17" s="2">
@@ -1108,11 +1120,11 @@
         <v>5</v>
       </c>
       <c r="H18" s="4">
-        <f>IDUs!H96</f>
+        <f>IDUs!L96</f>
         <v>20.059799999999999</v>
       </c>
       <c r="I18" s="2">
-        <f>IDUs!I96</f>
+        <f>IDUs!M96</f>
         <v>149.39206597274151</v>
       </c>
       <c r="J18" t="s">
@@ -1142,11 +1154,11 @@
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <f>IDUs!H99</f>
+        <f>IDUs!L99</f>
         <v>7.8960999999999997</v>
       </c>
       <c r="I19" s="2">
-        <f>IDUs!I99</f>
+        <f>IDUs!M99</f>
         <v>161.96</v>
       </c>
     </row>
@@ -1173,11 +1185,11 @@
         <v>1</v>
       </c>
       <c r="H20" s="4">
-        <f>IDUs!H102</f>
+        <f>IDUs!L102</f>
         <v>41.287700000000001</v>
       </c>
       <c r="I20" s="2">
-        <f>IDUs!I102</f>
+        <f>IDUs!M102</f>
         <v>538.92999999999995</v>
       </c>
       <c r="J20" t="s">
@@ -1220,11 +1232,11 @@
         <v>1</v>
       </c>
       <c r="H23" s="4">
-        <f>IDUs!H105/10000</f>
+        <f>IDUs!L105/10000</f>
         <v>5.0632999999999999</v>
       </c>
       <c r="I23" s="2">
-        <f>IDUs!I105</f>
+        <f>IDUs!M105</f>
         <v>5.81</v>
       </c>
       <c r="J23">
@@ -1257,11 +1269,11 @@
         <v>3</v>
       </c>
       <c r="H24" s="4">
-        <f>IDUs!H110</f>
+        <f>IDUs!L110</f>
         <v>21.9206</v>
       </c>
       <c r="I24" s="2">
-        <f>IDUs!I110</f>
+        <f>IDUs!M110</f>
         <v>11.960297756448274</v>
       </c>
       <c r="J24">
@@ -1294,11 +1306,11 @@
         <v>4</v>
       </c>
       <c r="H25" s="4">
-        <f>IDUs!H116</f>
+        <f>IDUs!L116</f>
         <v>35.7926</v>
       </c>
       <c r="I25" s="2">
-        <f>IDUs!I116</f>
+        <f>IDUs!M116</f>
         <v>29.066978341891897</v>
       </c>
       <c r="J25">
@@ -1331,11 +1343,11 @@
         <v>2</v>
       </c>
       <c r="H26" s="4">
-        <f>IDUs!H120</f>
+        <f>IDUs!L120</f>
         <v>28.562000000000001</v>
       </c>
       <c r="I26" s="2">
-        <f>IDUs!I120</f>
+        <f>IDUs!M120</f>
         <v>49.730076395210418</v>
       </c>
       <c r="J26">
@@ -1368,11 +1380,11 @@
         <v>3</v>
       </c>
       <c r="H27" s="4">
-        <f>IDUs!H125</f>
+        <f>IDUs!L125</f>
         <v>25.743200000000002</v>
       </c>
       <c r="I27" s="2">
-        <f>IDUs!I125</f>
+        <f>IDUs!M125</f>
         <v>53.512008685788857</v>
       </c>
       <c r="J27">
@@ -1405,11 +1417,11 @@
         <v>2</v>
       </c>
       <c r="H28" s="4">
-        <f>IDUs!H129</f>
+        <f>IDUs!L129</f>
         <v>14.622199999999999</v>
       </c>
       <c r="I28" s="2">
-        <f>IDUs!I129</f>
+        <f>IDUs!M129</f>
         <v>54.218883615324643</v>
       </c>
       <c r="J28">
@@ -1442,11 +1454,11 @@
         <v>6</v>
       </c>
       <c r="H29" s="4">
-        <f>IDUs!H137</f>
+        <f>IDUs!L137</f>
         <v>37.5364</v>
       </c>
       <c r="I29" s="2">
-        <f>IDUs!I137</f>
+        <f>IDUs!M137</f>
         <v>57.589091388625441</v>
       </c>
       <c r="J29">
@@ -1476,11 +1488,11 @@
         <v>1</v>
       </c>
       <c r="H30" s="4">
-        <f>IDUs!H139/10000</f>
+        <f>IDUs!L139/10000</f>
         <v>5.2785000000000002</v>
       </c>
       <c r="I30" s="2">
-        <f>IDUs!I139</f>
+        <f>IDUs!M139</f>
         <v>252.65</v>
       </c>
       <c r="J30">
@@ -1513,11 +1525,11 @@
         <v>1</v>
       </c>
       <c r="H31" s="4">
-        <f>IDUs!H140/10000</f>
+        <f>IDUs!L140/10000</f>
         <v>5.5853000000000002</v>
       </c>
       <c r="I31" s="2">
-        <f>IDUs!I140</f>
+        <f>IDUs!M140</f>
         <v>30.94</v>
       </c>
       <c r="J31">
@@ -1550,11 +1562,11 @@
         <v>1</v>
       </c>
       <c r="H32" s="4">
-        <f>IDUs!H141/10000</f>
+        <f>IDUs!L141/10000</f>
         <v>6.7222</v>
       </c>
       <c r="I32" s="2">
-        <f>IDUs!I141</f>
+        <f>IDUs!M141</f>
         <v>95.08</v>
       </c>
       <c r="J32">
@@ -1587,11 +1599,11 @@
         <v>1</v>
       </c>
       <c r="H33" s="4">
-        <f>IDUs!H142/10000</f>
+        <f>IDUs!L142/10000</f>
         <v>10.258800000000001</v>
       </c>
       <c r="I33" s="2">
-        <f>IDUs!I142</f>
+        <f>IDUs!M142</f>
         <v>86.9</v>
       </c>
       <c r="J33">
@@ -1624,11 +1636,11 @@
         <v>1</v>
       </c>
       <c r="H34" s="4">
-        <f>IDUs!H143/10000</f>
+        <f>IDUs!L143/10000</f>
         <v>6.5830000000000002</v>
       </c>
       <c r="I34" s="2">
-        <f>IDUs!I143</f>
+        <f>IDUs!M143</f>
         <v>665.6</v>
       </c>
       <c r="J34">
@@ -1914,22 +1926,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71514D07-858F-4F8F-B9B0-14D5E7A5141D}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:P143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="6" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1946,30 +1959,42 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1985,149 +2010,149 @@
       <c r="E3">
         <v>23765583</v>
       </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3">
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3">
         <v>37310</v>
       </c>
-      <c r="H3">
+      <c r="L3">
         <v>44172</v>
       </c>
-      <c r="I3" s="2">
+      <c r="M3" s="2">
         <v>113.24</v>
       </c>
-      <c r="J3">
-        <v>190</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N3">
+        <v>190</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D4">
         <v>2274</v>
       </c>
       <c r="E4">
         <v>23772703</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4">
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4">
         <v>37279</v>
       </c>
-      <c r="H4">
+      <c r="L4">
         <v>97565</v>
       </c>
-      <c r="I4" s="2">
+      <c r="M4" s="2">
         <v>114.32</v>
       </c>
-      <c r="J4">
-        <v>190</v>
-      </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>190</v>
+      </c>
+      <c r="O4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D5">
         <v>2251</v>
       </c>
       <c r="E5">
         <v>23772705</v>
       </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5">
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5">
         <v>36873</v>
       </c>
-      <c r="H5">
+      <c r="L5">
         <v>30567</v>
       </c>
-      <c r="I5" s="2">
+      <c r="M5" s="2">
         <v>115.07</v>
       </c>
-      <c r="J5">
-        <v>190</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>190</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D6">
         <v>2251</v>
       </c>
       <c r="E6">
         <v>23772705</v>
       </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6">
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6">
         <v>37240</v>
       </c>
-      <c r="H6">
+      <c r="L6">
         <v>23708</v>
       </c>
-      <c r="I6" s="2">
+      <c r="M6" s="2">
         <v>115.86</v>
       </c>
-      <c r="J6">
+      <c r="N6">
         <v>195</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D7">
         <v>2250</v>
       </c>
       <c r="E7">
         <v>23772713</v>
       </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7">
+      <c r="J7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7">
         <v>36850</v>
       </c>
-      <c r="H7">
+      <c r="L7">
         <v>45045</v>
       </c>
-      <c r="I7" s="2">
+      <c r="M7" s="2">
         <v>116.67</v>
       </c>
-      <c r="J7">
+      <c r="N7">
         <v>195</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G8" s="5" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="4">
-        <f>SUM(H3:H7)/10000</f>
+      <c r="L8" s="4">
+        <f>SUM(L3:L7)/10000</f>
         <v>24.105699999999999</v>
       </c>
-      <c r="I8" s="2">
-        <f>SUMPRODUCT(H3:H7,I3:I7)/(H8*10000)</f>
+      <c r="M8" s="2">
+        <f>SUMPRODUCT(L3:L7,M3:M7)/(L8*10000)</f>
         <v>114.80779151818864</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2143,68 +2168,68 @@
       <c r="E10">
         <v>23772709</v>
       </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10">
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10">
         <v>36786</v>
       </c>
-      <c r="H10">
+      <c r="L10">
         <v>71657</v>
       </c>
-      <c r="I10" s="2">
+      <c r="M10" s="2">
         <v>115.72</v>
       </c>
-      <c r="J10">
+      <c r="N10">
         <v>195</v>
       </c>
-      <c r="K10" t="s">
+      <c r="O10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D11">
         <v>2194</v>
       </c>
       <c r="E11">
         <v>23772709</v>
       </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11">
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11">
         <v>36776</v>
       </c>
-      <c r="H11">
+      <c r="L11">
         <v>56719</v>
       </c>
-      <c r="I11" s="2">
+      <c r="M11" s="2">
         <v>116.08</v>
       </c>
-      <c r="J11">
+      <c r="N11">
         <v>195</v>
       </c>
-      <c r="K11" t="s">
+      <c r="O11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G12" s="5" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="4">
-        <f>SUM(H10:H11)/10000</f>
+      <c r="L12" s="4">
+        <f>SUM(L10:L11)/10000</f>
         <v>12.8376</v>
       </c>
-      <c r="I12" s="2">
-        <f>SUMPRODUCT(H10:H11,I10:I11)/(H12*10000)</f>
+      <c r="M12" s="2">
+        <f>SUMPRODUCT(L10:L11,M10:M11)/(L12*10000)</f>
         <v>115.87905496354458</v>
       </c>
-      <c r="J12" t="s">
+      <c r="N12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2220,114 +2245,114 @@
       <c r="E14">
         <v>23772721</v>
       </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14">
+      <c r="J14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14">
         <v>36356</v>
       </c>
-      <c r="H14">
+      <c r="L14">
         <v>39502</v>
       </c>
-      <c r="I14" s="2">
+      <c r="M14" s="2">
         <v>117.98</v>
       </c>
-      <c r="J14">
-        <v>190</v>
-      </c>
-      <c r="K14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>190</v>
+      </c>
+      <c r="O14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>2198</v>
       </c>
       <c r="E15">
         <v>23774113</v>
       </c>
-      <c r="G15">
+      <c r="K15">
         <v>36324</v>
       </c>
-      <c r="H15">
+      <c r="L15">
         <v>81228</v>
       </c>
-      <c r="I15" s="2">
+      <c r="M15" s="2">
         <v>117.67</v>
       </c>
-      <c r="J15">
-        <v>190</v>
-      </c>
-      <c r="K15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>190</v>
+      </c>
+      <c r="O15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D16">
         <v>2194</v>
       </c>
       <c r="E16">
         <v>23772717</v>
       </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16">
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16">
         <v>36282</v>
       </c>
-      <c r="H16">
+      <c r="L16">
         <v>32023</v>
       </c>
-      <c r="I16" s="2">
+      <c r="M16" s="2">
         <v>118.28</v>
       </c>
-      <c r="J16">
-        <v>190</v>
-      </c>
-      <c r="K16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>190</v>
+      </c>
+      <c r="O16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D17">
         <v>2206</v>
       </c>
       <c r="E17">
         <v>23774111</v>
       </c>
-      <c r="G17">
+      <c r="K17">
         <v>36345</v>
       </c>
-      <c r="H17">
+      <c r="L17">
         <v>42644</v>
       </c>
-      <c r="I17" s="2">
+      <c r="M17" s="2">
         <v>118.42</v>
       </c>
-      <c r="J17">
-        <v>190</v>
-      </c>
-      <c r="K17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G18" s="5" t="s">
+      <c r="N17">
+        <v>190</v>
+      </c>
+      <c r="O17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="4">
-        <f>SUM(H14:H17)/10000</f>
+      <c r="L18" s="4">
+        <f>SUM(L14:L17)/10000</f>
         <v>19.5397</v>
       </c>
-      <c r="I18" s="2">
-        <f>SUMPRODUCT(H14:H17,I14:I17)/(H18*10000)</f>
+      <c r="M18" s="2">
+        <f>SUMPRODUCT(L14:L17,M14:M17)/(L18*10000)</f>
         <v>117.99632358736316</v>
       </c>
-      <c r="J18" t="s">
+      <c r="N18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2343,68 +2368,68 @@
       <c r="E20">
         <v>23772725</v>
       </c>
-      <c r="F20" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20">
+      <c r="J20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K20">
         <v>36305</v>
       </c>
-      <c r="H20">
+      <c r="L20">
         <v>30363</v>
       </c>
-      <c r="I20" s="2">
+      <c r="M20" s="2">
         <v>119.5</v>
       </c>
-      <c r="J20">
-        <v>190</v>
-      </c>
-      <c r="K20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>190</v>
+      </c>
+      <c r="O20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D21">
         <v>2069</v>
       </c>
       <c r="E21">
         <v>23772727</v>
       </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21">
+      <c r="J21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21">
         <v>36307</v>
       </c>
-      <c r="H21">
+      <c r="L21">
         <v>116500</v>
       </c>
-      <c r="I21" s="2">
+      <c r="M21" s="2">
         <v>120.72</v>
       </c>
-      <c r="J21">
-        <v>190</v>
-      </c>
-      <c r="K21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G22" s="5" t="s">
+      <c r="N21">
+        <v>190</v>
+      </c>
+      <c r="O21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="4">
-        <f>SUM(H20:H21)/10000</f>
+      <c r="L22" s="4">
+        <f>SUM(L20:L21)/10000</f>
         <v>14.686299999999999</v>
       </c>
-      <c r="I22" s="2">
-        <f>SUMPRODUCT(H20:H21,I20:I21)/(H22*10000)</f>
+      <c r="M22" s="2">
+        <f>SUMPRODUCT(L20:L21,M20:M21)/(L22*10000)</f>
         <v>120.46777268610882</v>
       </c>
-      <c r="J22" t="s">
+      <c r="N22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2420,100 +2445,100 @@
       <c r="E24">
         <v>23772727</v>
       </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24">
+      <c r="J24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24">
         <v>36255</v>
       </c>
-      <c r="H24">
+      <c r="L24">
         <v>250687</v>
       </c>
-      <c r="I24" s="2">
+      <c r="M24" s="2">
         <v>124.08</v>
       </c>
-      <c r="J24">
-        <v>190</v>
-      </c>
-      <c r="K24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="N24">
+        <v>190</v>
+      </c>
+      <c r="O24" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D25">
         <v>2069</v>
       </c>
       <c r="E25">
         <v>23772727</v>
       </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25">
+      <c r="J25" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25">
         <v>36228</v>
       </c>
-      <c r="H25">
+      <c r="L25">
         <v>36958</v>
       </c>
-      <c r="I25" s="2">
+      <c r="M25" s="2">
         <v>123.13</v>
       </c>
-      <c r="J25">
-        <v>190</v>
-      </c>
-      <c r="K25" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="N25">
+        <v>190</v>
+      </c>
+      <c r="O25" t="s">
+        <v>27</v>
+      </c>
+      <c r="P25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D26">
         <v>2069</v>
       </c>
       <c r="E26">
         <v>23772727</v>
       </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26">
+      <c r="J26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26">
         <v>36220</v>
       </c>
-      <c r="H26">
+      <c r="L26">
         <v>64343</v>
       </c>
-      <c r="I26" s="2">
+      <c r="M26" s="2">
         <v>124.78</v>
       </c>
-      <c r="J26">
-        <v>190</v>
-      </c>
-      <c r="K26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G27" s="5" t="s">
+      <c r="N26">
+        <v>190</v>
+      </c>
+      <c r="O26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="4">
-        <f>SUM(H24:H26)/10000</f>
+      <c r="L27" s="4">
+        <f>SUM(L24:L26)/10000</f>
         <v>35.198799999999999</v>
       </c>
-      <c r="I27" s="2">
-        <f>SUMPRODUCT(H24:H26,I24:I26)/(H27*10000)</f>
+      <c r="M27" s="2">
+        <f>SUMPRODUCT(L24:L26,M24:M26)/(L27*10000)</f>
         <v>124.10821118901781</v>
       </c>
-      <c r="J27" t="s">
+      <c r="N27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2529,42 +2554,42 @@
       <c r="E29">
         <v>23772727</v>
       </c>
-      <c r="F29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29">
+      <c r="J29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29">
         <v>35846</v>
       </c>
-      <c r="H29">
+      <c r="L29">
         <v>141017</v>
       </c>
-      <c r="I29" s="2">
+      <c r="M29" s="2">
         <v>122.91</v>
       </c>
-      <c r="J29">
-        <v>190</v>
-      </c>
-      <c r="K29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G30" s="5" t="s">
+      <c r="N29">
+        <v>190</v>
+      </c>
+      <c r="O29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="4">
-        <f>SUM(H29:H29)/10000</f>
+      <c r="L30" s="4">
+        <f>SUM(L29:L29)/10000</f>
         <v>14.101699999999999</v>
       </c>
-      <c r="I30" s="2">
-        <f>SUMPRODUCT(H29:H29,I29:I29)/(H30*10000)</f>
+      <c r="M30" s="2">
+        <f>SUMPRODUCT(L29:L29,M29:M29)/(L30*10000)</f>
         <v>122.91</v>
       </c>
-      <c r="J30" t="s">
+      <c r="N30" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2580,140 +2605,140 @@
       <c r="E32">
         <v>23772727</v>
       </c>
-      <c r="F32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32">
+      <c r="J32" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32">
         <v>35767</v>
       </c>
-      <c r="H32">
+      <c r="L32">
         <v>137221</v>
       </c>
-      <c r="I32" s="2">
+      <c r="M32" s="2">
         <v>123.88</v>
       </c>
-      <c r="J32">
-        <v>190</v>
-      </c>
-      <c r="K32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>190</v>
+      </c>
+      <c r="O32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D33">
         <v>2122</v>
       </c>
       <c r="E33">
         <v>23772729</v>
       </c>
-      <c r="F33" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33">
+      <c r="J33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33">
         <v>35332</v>
       </c>
-      <c r="H33">
+      <c r="L33">
         <v>75379</v>
       </c>
-      <c r="I33" s="2">
+      <c r="M33" s="2">
         <v>126.88</v>
       </c>
-      <c r="J33">
-        <v>190</v>
-      </c>
-      <c r="K33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N33">
+        <v>190</v>
+      </c>
+      <c r="O33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D34">
         <v>2004</v>
       </c>
       <c r="E34">
         <v>23774181</v>
       </c>
-      <c r="G34">
+      <c r="K34">
         <v>35244</v>
       </c>
-      <c r="H34">
+      <c r="L34">
         <v>28533</v>
       </c>
-      <c r="I34" s="2">
+      <c r="M34" s="2">
         <v>127.06</v>
       </c>
-      <c r="J34">
-        <v>190</v>
-      </c>
-      <c r="K34" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N34">
+        <v>190</v>
+      </c>
+      <c r="O34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D35">
         <v>2037</v>
       </c>
       <c r="E35">
         <v>23772731</v>
       </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35">
+      <c r="J35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35">
         <v>35243</v>
       </c>
-      <c r="H35">
+      <c r="L35">
         <v>44085</v>
       </c>
-      <c r="I35" s="2">
+      <c r="M35" s="2">
         <v>125.35</v>
       </c>
-      <c r="J35">
-        <v>190</v>
-      </c>
-      <c r="K35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N35">
+        <v>190</v>
+      </c>
+      <c r="O35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D36">
         <v>2004</v>
       </c>
       <c r="E36">
         <v>23774181</v>
       </c>
-      <c r="G36">
+      <c r="K36">
         <v>35233</v>
       </c>
-      <c r="H36">
+      <c r="L36">
         <v>45898</v>
       </c>
-      <c r="I36" s="2">
+      <c r="M36" s="2">
         <v>126.24</v>
       </c>
-      <c r="J36">
-        <v>190</v>
-      </c>
-      <c r="K36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G37" s="5" t="s">
+      <c r="N36">
+        <v>190</v>
+      </c>
+      <c r="O36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="4">
-        <f>SUM(H32:H36)/10000</f>
+      <c r="L37" s="4">
+        <f>SUM(L32:L36)/10000</f>
         <v>33.111600000000003</v>
       </c>
-      <c r="I37" s="2">
-        <f>SUMPRODUCT(H32:H36,I32:I36)/(H37*10000)</f>
+      <c r="M37" s="2">
+        <f>SUMPRODUCT(L32:L36,M32:M36)/(L37*10000)</f>
         <v>125.35983235482429</v>
       </c>
-      <c r="J37" t="s">
+      <c r="N37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2729,39 +2754,39 @@
       <c r="E39">
         <v>23774181</v>
       </c>
-      <c r="G39">
+      <c r="K39">
         <v>34761</v>
       </c>
-      <c r="H39">
+      <c r="L39">
         <v>104520</v>
       </c>
-      <c r="I39" s="2">
+      <c r="M39" s="2">
         <v>128.61000000000001</v>
       </c>
-      <c r="J39">
-        <v>190</v>
-      </c>
-      <c r="K39" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G40" s="5" t="s">
+      <c r="N39">
+        <v>190</v>
+      </c>
+      <c r="O39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="4">
-        <f>SUM(H39:H39)/10000</f>
+      <c r="L40" s="4">
+        <f>SUM(L39:L39)/10000</f>
         <v>10.452</v>
       </c>
-      <c r="I40" s="2">
-        <f>SUMPRODUCT(H39:H39,I39:I39)/(H40*10000)</f>
+      <c r="M40" s="2">
+        <f>SUMPRODUCT(L39:L39,M39:M39)/(L40*10000)</f>
         <v>128.61000000000001</v>
       </c>
-      <c r="J40" t="s">
+      <c r="N40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2777,94 +2802,94 @@
       <c r="E42">
         <v>23772731</v>
       </c>
-      <c r="F42" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42">
+      <c r="J42" t="s">
+        <v>7</v>
+      </c>
+      <c r="K42">
         <v>34773</v>
       </c>
-      <c r="H42">
+      <c r="L42">
         <v>149305</v>
       </c>
-      <c r="I42" s="2">
+      <c r="M42" s="2">
         <v>128.71</v>
       </c>
-      <c r="J42">
-        <v>190</v>
-      </c>
-      <c r="K42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N42">
+        <v>190</v>
+      </c>
+      <c r="O42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D43">
         <v>2037</v>
       </c>
       <c r="E43">
         <v>23772731</v>
       </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43">
+      <c r="J43" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43">
         <v>34764</v>
       </c>
-      <c r="H43">
+      <c r="L43">
         <v>134530</v>
       </c>
-      <c r="I43" s="2">
+      <c r="M43" s="2">
         <v>128.31</v>
       </c>
-      <c r="J43">
-        <v>190</v>
-      </c>
-      <c r="K43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>190</v>
+      </c>
+      <c r="O43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D44">
         <v>2037</v>
       </c>
       <c r="E44">
         <v>23772731</v>
       </c>
-      <c r="F44" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44">
+      <c r="J44" t="s">
+        <v>7</v>
+      </c>
+      <c r="K44">
         <v>34344</v>
       </c>
-      <c r="H44">
+      <c r="L44">
         <v>24108</v>
       </c>
-      <c r="I44" s="2">
+      <c r="M44" s="2">
         <v>130.30000000000001</v>
       </c>
-      <c r="J44">
-        <v>190</v>
-      </c>
-      <c r="K44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G45" s="5" t="s">
+      <c r="N44">
+        <v>190</v>
+      </c>
+      <c r="O44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="4">
-        <f>SUM(H42:H44)/10000</f>
+      <c r="L45" s="4">
+        <f>SUM(L42:L44)/10000</f>
         <v>30.7943</v>
       </c>
-      <c r="I45" s="2">
-        <f>SUMPRODUCT(H42:H44,I42:I44)/(H45*10000)</f>
+      <c r="M45" s="2">
+        <f>SUMPRODUCT(L42:L44,M42:M44)/(L45*10000)</f>
         <v>128.65973004744384</v>
       </c>
-      <c r="J45" t="s">
+      <c r="N45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2880,68 +2905,68 @@
       <c r="E47">
         <v>23772737</v>
       </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47">
+      <c r="J47" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47">
         <v>33827</v>
       </c>
-      <c r="H47">
+      <c r="L47">
         <v>41473</v>
       </c>
-      <c r="I47" s="2">
+      <c r="M47" s="2">
         <v>132.80000000000001</v>
       </c>
-      <c r="J47">
-        <v>190</v>
-      </c>
-      <c r="K47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N47">
+        <v>190</v>
+      </c>
+      <c r="O47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D48">
         <v>2033</v>
       </c>
       <c r="E48">
         <v>23772737</v>
       </c>
-      <c r="F48" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48">
+      <c r="J48" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48">
         <v>33807</v>
       </c>
-      <c r="H48">
+      <c r="L48">
         <v>43240</v>
       </c>
-      <c r="I48" s="2">
+      <c r="M48" s="2">
         <v>130.38</v>
       </c>
-      <c r="J48">
-        <v>190</v>
-      </c>
-      <c r="K48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G49" s="5" t="s">
+      <c r="N48">
+        <v>190</v>
+      </c>
+      <c r="O48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K49" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H49" s="4">
-        <f>SUM(H47:H48)/10000</f>
+      <c r="L49" s="4">
+        <f>SUM(L47:L48)/10000</f>
         <v>8.4712999999999994</v>
       </c>
-      <c r="I49" s="2">
-        <f>SUMPRODUCT(H47:H48,I47:I48)/(H49*10000)</f>
+      <c r="M49" s="2">
+        <f>SUMPRODUCT(L47:L48,M47:M48)/(L49*10000)</f>
         <v>131.56476101660903</v>
       </c>
-      <c r="J49" t="s">
+      <c r="N49" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>11</v>
       </c>
@@ -2957,172 +2982,172 @@
       <c r="E51">
         <v>23772739</v>
       </c>
-      <c r="F51" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51">
+      <c r="J51" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51">
         <v>33362</v>
       </c>
-      <c r="H51">
+      <c r="L51">
         <v>41477</v>
       </c>
-      <c r="I51" s="2">
+      <c r="M51" s="2">
         <v>129.62</v>
       </c>
-      <c r="J51">
-        <v>190</v>
-      </c>
-      <c r="K51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N51">
+        <v>190</v>
+      </c>
+      <c r="O51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D52">
         <v>2005</v>
       </c>
       <c r="E52">
         <v>23772739</v>
       </c>
-      <c r="F52" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52">
+      <c r="J52" t="s">
+        <v>7</v>
+      </c>
+      <c r="K52">
         <v>33323</v>
       </c>
-      <c r="H52">
+      <c r="L52">
         <v>54647</v>
       </c>
-      <c r="I52" s="2">
+      <c r="M52" s="2">
         <v>130.16</v>
       </c>
-      <c r="J52">
-        <v>190</v>
-      </c>
-      <c r="K52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N52">
+        <v>190</v>
+      </c>
+      <c r="O52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D53">
         <v>1966</v>
       </c>
       <c r="E53">
         <v>23772741</v>
       </c>
-      <c r="F53" t="s">
-        <v>7</v>
-      </c>
-      <c r="G53">
+      <c r="J53" t="s">
+        <v>7</v>
+      </c>
+      <c r="K53">
         <v>33303</v>
       </c>
-      <c r="H53">
+      <c r="L53">
         <v>33230</v>
       </c>
-      <c r="I53" s="2">
+      <c r="M53" s="2">
         <v>130.08000000000001</v>
       </c>
-      <c r="J53">
-        <v>190</v>
-      </c>
-      <c r="K53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N53">
+        <v>190</v>
+      </c>
+      <c r="O53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D54">
         <v>1966</v>
       </c>
       <c r="E54">
         <v>23772741</v>
       </c>
-      <c r="F54" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54">
+      <c r="J54" t="s">
+        <v>7</v>
+      </c>
+      <c r="K54">
         <v>33310</v>
       </c>
-      <c r="H54">
+      <c r="L54">
         <v>149289</v>
       </c>
-      <c r="I54" s="2">
+      <c r="M54" s="2">
         <v>130.51</v>
       </c>
-      <c r="J54">
-        <v>190</v>
-      </c>
-      <c r="K54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N54">
+        <v>190</v>
+      </c>
+      <c r="O54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D55">
         <v>1966</v>
       </c>
       <c r="E55">
         <v>23772741</v>
       </c>
-      <c r="F55" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55">
+      <c r="J55" t="s">
+        <v>7</v>
+      </c>
+      <c r="K55">
         <v>33349</v>
       </c>
-      <c r="H55">
+      <c r="L55">
         <v>59644</v>
       </c>
-      <c r="I55" s="2">
+      <c r="M55" s="2">
         <v>131.46</v>
       </c>
-      <c r="J55">
-        <v>190</v>
-      </c>
-      <c r="K55" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N55">
+        <v>190</v>
+      </c>
+      <c r="O55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D56">
         <v>2005</v>
       </c>
       <c r="E56">
         <v>23772739</v>
       </c>
-      <c r="F56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G56">
+      <c r="J56" t="s">
+        <v>7</v>
+      </c>
+      <c r="K56">
         <v>33724</v>
       </c>
-      <c r="H56">
+      <c r="L56">
         <v>28116</v>
       </c>
-      <c r="I56" s="2">
+      <c r="M56" s="2">
         <v>132.88999999999999</v>
       </c>
-      <c r="J56">
-        <v>190</v>
-      </c>
-      <c r="K56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G57" s="5" t="s">
+      <c r="N56">
+        <v>190</v>
+      </c>
+      <c r="O56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H57" s="4">
-        <f>SUM(H51:H56)/10000</f>
+      <c r="L57" s="4">
+        <f>SUM(L51:L56)/10000</f>
         <v>36.640300000000003</v>
       </c>
-      <c r="I57" s="2">
-        <f>SUMPRODUCT(H51:H56,I51:I56)/(H57*10000)</f>
+      <c r="M57" s="2">
+        <f>SUMPRODUCT(L51:L56,M51:M56)/(L57*10000)</f>
         <v>130.65532632101809</v>
       </c>
-      <c r="J57" t="s">
+      <c r="N57" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>12</v>
       </c>
@@ -3138,143 +3163,143 @@
       <c r="E59">
         <v>23772743</v>
       </c>
-      <c r="F59" t="s">
-        <v>7</v>
-      </c>
-      <c r="G59">
+      <c r="J59" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59">
         <v>32813</v>
       </c>
-      <c r="H59">
+      <c r="L59">
         <v>23559</v>
       </c>
-      <c r="I59" s="2">
+      <c r="M59" s="2">
         <v>135</v>
       </c>
-      <c r="J59">
-        <v>190</v>
-      </c>
-      <c r="K59" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N59">
+        <v>190</v>
+      </c>
+      <c r="O59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D60">
         <v>1972</v>
       </c>
       <c r="E60">
         <v>23774285</v>
       </c>
-      <c r="G60">
+      <c r="K60">
         <v>32865</v>
       </c>
-      <c r="H60">
+      <c r="L60">
         <v>53187</v>
       </c>
-      <c r="I60" s="2">
+      <c r="M60" s="2">
         <v>134.47999999999999</v>
       </c>
-      <c r="J60">
-        <v>190</v>
-      </c>
-      <c r="K60" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N60">
+        <v>190</v>
+      </c>
+      <c r="O60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D61">
         <v>1946</v>
       </c>
       <c r="E61">
         <v>23772745</v>
       </c>
-      <c r="F61" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61">
+      <c r="J61" t="s">
+        <v>7</v>
+      </c>
+      <c r="K61">
         <v>33278</v>
       </c>
-      <c r="H61">
+      <c r="L61">
         <v>80665</v>
       </c>
-      <c r="I61" s="2">
+      <c r="M61" s="2">
         <v>133.43</v>
       </c>
-      <c r="J61">
-        <v>190</v>
-      </c>
-      <c r="K61" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N61">
+        <v>190</v>
+      </c>
+      <c r="O61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D62">
         <v>1972</v>
       </c>
       <c r="E62">
         <v>23774285</v>
       </c>
-      <c r="G62">
+      <c r="K62">
         <v>33262</v>
       </c>
-      <c r="H62">
+      <c r="L62">
         <v>23268</v>
       </c>
-      <c r="I62" s="3">
+      <c r="M62" s="3">
         <v>0</v>
       </c>
-      <c r="J62">
-        <v>190</v>
-      </c>
-      <c r="K62" t="s">
-        <v>27</v>
-      </c>
-      <c r="L62" t="s">
+      <c r="N62">
+        <v>190</v>
+      </c>
+      <c r="O62" t="s">
+        <v>27</v>
+      </c>
+      <c r="P62" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D63">
         <v>1946</v>
       </c>
       <c r="E63">
         <v>23772745</v>
       </c>
-      <c r="F63" t="s">
-        <v>7</v>
-      </c>
-      <c r="G63">
+      <c r="J63" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63">
         <v>33324</v>
       </c>
-      <c r="H63">
+      <c r="L63">
         <v>82089</v>
       </c>
-      <c r="I63" s="2">
+      <c r="M63" s="2">
         <v>134.77000000000001</v>
       </c>
-      <c r="J63">
-        <v>190</v>
-      </c>
-      <c r="K63" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G64" s="5" t="s">
+      <c r="N63">
+        <v>190</v>
+      </c>
+      <c r="O63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K64" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H64" s="4">
-        <f>SUM(H59:H63)/10000</f>
+      <c r="L64" s="4">
+        <f>SUM(L59:L63)/10000</f>
         <v>26.276800000000001</v>
       </c>
-      <c r="I64" s="3">
-        <f>SUMPRODUCT(H59:H63,I59:I63)/((H64-H62/10000)*10000)</f>
+      <c r="M64" s="3">
+        <f>SUMPRODUCT(L59:L63,M59:M63)/((L64-L62/10000)*10000)</f>
         <v>134.27690288100209</v>
       </c>
-      <c r="J64" t="s">
+      <c r="N64" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>13</v>
       </c>
@@ -3290,42 +3315,42 @@
       <c r="E66">
         <v>23772745</v>
       </c>
-      <c r="F66" t="s">
-        <v>7</v>
-      </c>
-      <c r="G66">
+      <c r="J66" t="s">
+        <v>7</v>
+      </c>
+      <c r="K66">
         <v>33306</v>
       </c>
-      <c r="H66">
+      <c r="L66">
         <v>65332</v>
       </c>
-      <c r="I66" s="2">
+      <c r="M66" s="2">
         <v>134.74</v>
       </c>
-      <c r="J66">
-        <v>190</v>
-      </c>
-      <c r="K66" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G67" s="5" t="s">
+      <c r="N66">
+        <v>190</v>
+      </c>
+      <c r="O66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K67" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H67" s="4">
-        <f>SUM(H66:H66)/10000</f>
+      <c r="L67" s="4">
+        <f>SUM(L66:L66)/10000</f>
         <v>6.5331999999999999</v>
       </c>
-      <c r="I67" s="2">
-        <f>SUMPRODUCT(H66:H66,I66:I66)/(H67*10000)</f>
+      <c r="M67" s="2">
+        <f>SUMPRODUCT(L66:L66,M66:M66)/(L67*10000)</f>
         <v>134.74</v>
       </c>
-      <c r="J67" t="s">
+      <c r="N67" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>14</v>
       </c>
@@ -3341,42 +3366,42 @@
       <c r="E69">
         <v>23772745</v>
       </c>
-      <c r="F69" t="s">
-        <v>7</v>
-      </c>
-      <c r="G69">
+      <c r="J69" t="s">
+        <v>7</v>
+      </c>
+      <c r="K69">
         <v>33803</v>
       </c>
-      <c r="H69">
+      <c r="L69">
         <v>154578</v>
       </c>
-      <c r="I69" s="2">
+      <c r="M69" s="2">
         <v>139.35</v>
       </c>
-      <c r="J69">
-        <v>190</v>
-      </c>
-      <c r="K69" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G70" s="5" t="s">
+      <c r="N69">
+        <v>190</v>
+      </c>
+      <c r="O69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K70" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H70" s="4">
-        <f>SUM(H69:H69)/10000</f>
+      <c r="L70" s="4">
+        <f>SUM(L69:L69)/10000</f>
         <v>15.457800000000001</v>
       </c>
-      <c r="I70" s="2">
-        <f>SUMPRODUCT(H69:H69,I69:I69)/(H70*10000)</f>
+      <c r="M70" s="2">
+        <f>SUMPRODUCT(L69:L69,M69:M69)/(L70*10000)</f>
         <v>139.35</v>
       </c>
-      <c r="J70" t="s">
+      <c r="N70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -3392,458 +3417,486 @@
       <c r="E72">
         <v>23772753</v>
       </c>
-      <c r="F72" t="s">
-        <v>7</v>
-      </c>
-      <c r="G72">
+      <c r="F72">
+        <v>448.31</v>
+      </c>
+      <c r="G72" s="2">
+        <f>F72*0.3048</f>
+        <v>136.64488800000001</v>
+      </c>
+      <c r="H72" s="2">
+        <v>459.91</v>
+      </c>
+      <c r="I72" s="2">
+        <f>H72*0.3048</f>
+        <v>140.18056800000002</v>
+      </c>
+      <c r="J72" t="s">
+        <v>7</v>
+      </c>
+      <c r="K72">
+        <v>32345</v>
+      </c>
+      <c r="L72">
+        <v>49169</v>
+      </c>
+      <c r="M72" s="2">
+        <v>140.29</v>
+      </c>
+      <c r="N72">
+        <v>190</v>
+      </c>
+      <c r="O72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>1928</v>
+      </c>
+      <c r="E73">
+        <v>23772755</v>
+      </c>
+      <c r="J73" t="s">
+        <v>7</v>
+      </c>
+      <c r="K73">
+        <v>32289</v>
+      </c>
+      <c r="L73">
+        <v>81849</v>
+      </c>
+      <c r="M73" s="2">
+        <v>141.33000000000001</v>
+      </c>
+      <c r="N73">
+        <v>190</v>
+      </c>
+      <c r="O73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>1821</v>
+      </c>
+      <c r="E74">
+        <v>23772759</v>
+      </c>
+      <c r="J74" t="s">
+        <v>7</v>
+      </c>
+      <c r="K74">
+        <v>32250</v>
+      </c>
+      <c r="L74">
+        <v>115890</v>
+      </c>
+      <c r="M74" s="2">
+        <v>141.88999999999999</v>
+      </c>
+      <c r="N74">
+        <v>190</v>
+      </c>
+      <c r="O74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>1941</v>
+      </c>
+      <c r="E75">
+        <v>23772757</v>
+      </c>
+      <c r="J75" t="s">
+        <v>7</v>
+      </c>
+      <c r="K75">
+        <v>32280</v>
+      </c>
+      <c r="L75">
+        <v>82100</v>
+      </c>
+      <c r="M75" s="2">
+        <v>141.9</v>
+      </c>
+      <c r="N75">
+        <v>190</v>
+      </c>
+      <c r="O75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>1939</v>
+      </c>
+      <c r="E76">
+        <v>23772753</v>
+      </c>
+      <c r="J76" t="s">
+        <v>7</v>
+      </c>
+      <c r="K76">
         <v>32743</v>
       </c>
-      <c r="H72">
+      <c r="L76">
         <v>116029</v>
       </c>
-      <c r="I72" s="2">
+      <c r="M76" s="2">
         <v>142.27000000000001</v>
       </c>
-      <c r="J72">
-        <v>190</v>
-      </c>
-      <c r="K72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D73">
+      <c r="N76">
+        <v>190</v>
+      </c>
+      <c r="O76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>1821</v>
+      </c>
+      <c r="E77">
+        <v>23772759</v>
+      </c>
+      <c r="J77" t="s">
+        <v>7</v>
+      </c>
+      <c r="K77">
+        <v>31837</v>
+      </c>
+      <c r="L77">
+        <v>404169</v>
+      </c>
+      <c r="M77" s="2">
+        <v>142.29</v>
+      </c>
+      <c r="N77">
+        <v>190</v>
+      </c>
+      <c r="O77" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>1821</v>
+      </c>
+      <c r="E78">
+        <v>23772759</v>
+      </c>
+      <c r="J78" t="s">
+        <v>7</v>
+      </c>
+      <c r="K78">
+        <v>32193</v>
+      </c>
+      <c r="L78">
+        <v>57042</v>
+      </c>
+      <c r="M78" s="2">
+        <v>142.56</v>
+      </c>
+      <c r="N78">
+        <v>190</v>
+      </c>
+      <c r="O78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>1928</v>
+      </c>
+      <c r="E79">
+        <v>23772755</v>
+      </c>
+      <c r="J79" t="s">
+        <v>7</v>
+      </c>
+      <c r="K79">
+        <v>32312</v>
+      </c>
+      <c r="L79">
+        <v>39872</v>
+      </c>
+      <c r="M79" s="2">
+        <v>142.86000000000001</v>
+      </c>
+      <c r="N79">
+        <v>190</v>
+      </c>
+      <c r="O79" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>1909</v>
+      </c>
+      <c r="E80">
+        <v>23772761</v>
+      </c>
+      <c r="J80" t="s">
+        <v>7</v>
+      </c>
+      <c r="K80">
+        <v>31796</v>
+      </c>
+      <c r="L80">
+        <v>29765</v>
+      </c>
+      <c r="M80" s="2">
+        <v>143.07</v>
+      </c>
+      <c r="N80">
+        <v>190</v>
+      </c>
+      <c r="O80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D81">
         <v>1939</v>
       </c>
-      <c r="E73">
+      <c r="E81">
         <v>23772753</v>
       </c>
-      <c r="F73" t="s">
-        <v>7</v>
-      </c>
-      <c r="G73">
+      <c r="J81" t="s">
+        <v>7</v>
+      </c>
+      <c r="K81">
         <v>32723</v>
       </c>
-      <c r="H73">
+      <c r="L81">
         <v>153748</v>
       </c>
-      <c r="I73" s="2">
+      <c r="M81" s="2">
         <v>144.02000000000001</v>
       </c>
-      <c r="J73">
-        <v>190</v>
-      </c>
-      <c r="K73" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D74">
-        <v>1939</v>
-      </c>
-      <c r="E74">
-        <v>23772753</v>
-      </c>
-      <c r="F74" t="s">
-        <v>7</v>
-      </c>
-      <c r="G74">
-        <v>32345</v>
-      </c>
-      <c r="H74">
-        <v>49169</v>
-      </c>
-      <c r="I74" s="2">
-        <v>140.29</v>
-      </c>
-      <c r="J74">
-        <v>190</v>
-      </c>
-      <c r="K74" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D75">
-        <v>1928</v>
-      </c>
-      <c r="E75">
-        <v>23772755</v>
-      </c>
-      <c r="F75" t="s">
-        <v>7</v>
-      </c>
-      <c r="G75">
-        <v>32312</v>
-      </c>
-      <c r="H75">
-        <v>39872</v>
-      </c>
-      <c r="I75" s="2">
-        <v>142.86000000000001</v>
-      </c>
-      <c r="J75">
-        <v>190</v>
-      </c>
-      <c r="K75" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D76">
-        <v>1928</v>
-      </c>
-      <c r="E76">
-        <v>23772755</v>
-      </c>
-      <c r="F76" t="s">
-        <v>7</v>
-      </c>
-      <c r="G76">
-        <v>32293</v>
-      </c>
-      <c r="H76">
-        <v>44564</v>
-      </c>
-      <c r="I76" s="2">
-        <v>144.02000000000001</v>
-      </c>
-      <c r="J76">
-        <v>190</v>
-      </c>
-      <c r="K76" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D77">
-        <v>1928</v>
-      </c>
-      <c r="E77">
-        <v>23772755</v>
-      </c>
-      <c r="F77" t="s">
-        <v>7</v>
-      </c>
-      <c r="G77">
-        <v>32289</v>
-      </c>
-      <c r="H77">
-        <v>81849</v>
-      </c>
-      <c r="I77" s="2">
-        <v>141.33000000000001</v>
-      </c>
-      <c r="J77">
-        <v>190</v>
-      </c>
-      <c r="K77" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D78">
-        <v>1941</v>
-      </c>
-      <c r="E78">
-        <v>23772757</v>
-      </c>
-      <c r="F78" t="s">
-        <v>7</v>
-      </c>
-      <c r="G78">
-        <v>32280</v>
-      </c>
-      <c r="H78">
-        <v>82100</v>
-      </c>
-      <c r="I78" s="2">
-        <v>141.9</v>
-      </c>
-      <c r="J78">
-        <v>190</v>
-      </c>
-      <c r="K78" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D79">
-        <v>1821</v>
-      </c>
-      <c r="E79">
-        <v>23772759</v>
-      </c>
-      <c r="F79" t="s">
-        <v>7</v>
-      </c>
-      <c r="G79">
-        <v>32250</v>
-      </c>
-      <c r="H79">
-        <v>115890</v>
-      </c>
-      <c r="I79" s="2">
-        <v>141.88999999999999</v>
-      </c>
-      <c r="J79">
-        <v>190</v>
-      </c>
-      <c r="K79" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D80">
-        <v>1821</v>
-      </c>
-      <c r="E80">
-        <v>23772759</v>
-      </c>
-      <c r="F80" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80">
-        <v>32193</v>
-      </c>
-      <c r="H80">
-        <v>57042</v>
-      </c>
-      <c r="I80" s="2">
-        <v>142.56</v>
-      </c>
-      <c r="J80">
-        <v>190</v>
-      </c>
-      <c r="K80" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D81">
-        <v>1928</v>
-      </c>
-      <c r="E81">
-        <v>23772755</v>
-      </c>
-      <c r="F81" t="s">
-        <v>7</v>
-      </c>
-      <c r="G81">
-        <v>32245</v>
-      </c>
-      <c r="H81">
-        <v>44971</v>
-      </c>
-      <c r="I81" s="2">
-        <v>145.02000000000001</v>
-      </c>
-      <c r="J81">
-        <v>190</v>
-      </c>
-      <c r="K81" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N81">
+        <v>190</v>
+      </c>
+      <c r="O81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D82">
         <v>1928</v>
       </c>
       <c r="E82">
         <v>23772755</v>
       </c>
-      <c r="F82" t="s">
-        <v>7</v>
-      </c>
-      <c r="G82">
+      <c r="J82" t="s">
+        <v>7</v>
+      </c>
+      <c r="K82">
+        <v>32293</v>
+      </c>
+      <c r="L82">
+        <v>44564</v>
+      </c>
+      <c r="M82" s="2">
+        <v>144.02000000000001</v>
+      </c>
+      <c r="N82">
+        <v>190</v>
+      </c>
+      <c r="O82" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>1848</v>
+      </c>
+      <c r="E83">
+        <v>23772763</v>
+      </c>
+      <c r="J83" t="s">
+        <v>7</v>
+      </c>
+      <c r="K83">
+        <v>31811</v>
+      </c>
+      <c r="L83">
+        <v>142161</v>
+      </c>
+      <c r="M83" s="2">
+        <v>144.25</v>
+      </c>
+      <c r="N83">
+        <v>190</v>
+      </c>
+      <c r="O83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>1928</v>
+      </c>
+      <c r="E84">
+        <v>23772755</v>
+      </c>
+      <c r="J84" t="s">
+        <v>7</v>
+      </c>
+      <c r="K84">
         <v>32286</v>
       </c>
-      <c r="H82">
+      <c r="L84">
         <v>55945</v>
       </c>
-      <c r="I82" s="2">
+      <c r="M84" s="2">
         <v>145</v>
       </c>
-      <c r="J82">
-        <v>190</v>
-      </c>
-      <c r="K82" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D83">
+      <c r="N84">
+        <v>190</v>
+      </c>
+      <c r="O84" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D85">
         <v>1928</v>
       </c>
-      <c r="E83">
+      <c r="E85">
         <v>23772755</v>
       </c>
-      <c r="F83" t="s">
-        <v>7</v>
-      </c>
-      <c r="G83">
+      <c r="J85" t="s">
+        <v>7</v>
+      </c>
+      <c r="K85">
+        <v>32245</v>
+      </c>
+      <c r="L85">
+        <v>44971</v>
+      </c>
+      <c r="M85" s="2">
+        <v>145.02000000000001</v>
+      </c>
+      <c r="N85">
+        <v>190</v>
+      </c>
+      <c r="O85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>1848</v>
+      </c>
+      <c r="E86">
+        <v>23772763</v>
+      </c>
+      <c r="J86" t="s">
+        <v>7</v>
+      </c>
+      <c r="K86">
+        <v>31703</v>
+      </c>
+      <c r="L86">
+        <v>46987</v>
+      </c>
+      <c r="M86" s="2">
+        <v>145.16999999999999</v>
+      </c>
+      <c r="N86">
+        <v>190</v>
+      </c>
+      <c r="O86" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>1777</v>
+      </c>
+      <c r="E87">
+        <v>23772765</v>
+      </c>
+      <c r="J87" t="s">
+        <v>7</v>
+      </c>
+      <c r="K87">
+        <v>32208</v>
+      </c>
+      <c r="L87">
+        <v>112978</v>
+      </c>
+      <c r="M87" s="2">
+        <v>145.49</v>
+      </c>
+      <c r="N87">
+        <v>190</v>
+      </c>
+      <c r="O87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>1928</v>
+      </c>
+      <c r="E88">
+        <v>23772755</v>
+      </c>
+      <c r="F88">
+        <v>456.51</v>
+      </c>
+      <c r="G88" s="2">
+        <f>F88*0.3048</f>
+        <v>139.144248</v>
+      </c>
+      <c r="H88">
+        <v>459.54</v>
+      </c>
+      <c r="I88" s="2">
+        <f>H88*0.3048</f>
+        <v>140.06779200000003</v>
+      </c>
+      <c r="J88" t="s">
+        <v>7</v>
+      </c>
+      <c r="K88">
         <v>32225</v>
       </c>
-      <c r="H83">
+      <c r="L88">
         <v>40802</v>
       </c>
-      <c r="I83" s="2">
+      <c r="M88" s="2">
         <v>145.81</v>
       </c>
-      <c r="J83">
-        <v>190</v>
-      </c>
-      <c r="K83" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D84">
-        <v>1777</v>
-      </c>
-      <c r="E84">
-        <v>23772765</v>
-      </c>
-      <c r="F84" t="s">
-        <v>7</v>
-      </c>
-      <c r="G84">
-        <v>32208</v>
-      </c>
-      <c r="H84">
-        <v>112978</v>
-      </c>
-      <c r="I84" s="2">
-        <v>145.49</v>
-      </c>
-      <c r="J84">
-        <v>190</v>
-      </c>
-      <c r="K84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D85">
-        <v>1848</v>
-      </c>
-      <c r="E85">
-        <v>23772763</v>
-      </c>
-      <c r="F85" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85">
-        <v>31811</v>
-      </c>
-      <c r="H85">
-        <v>142161</v>
-      </c>
-      <c r="I85" s="2">
-        <v>144.25</v>
-      </c>
-      <c r="J85">
-        <v>190</v>
-      </c>
-      <c r="K85" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D86">
-        <v>1909</v>
-      </c>
-      <c r="E86">
-        <v>23772761</v>
-      </c>
-      <c r="F86" t="s">
-        <v>7</v>
-      </c>
-      <c r="G86">
-        <v>31796</v>
-      </c>
-      <c r="H86">
-        <v>29765</v>
-      </c>
-      <c r="I86" s="2">
-        <v>143.07</v>
-      </c>
-      <c r="J86">
-        <v>190</v>
-      </c>
-      <c r="K86" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D87">
-        <v>1821</v>
-      </c>
-      <c r="E87">
-        <v>23772759</v>
-      </c>
-      <c r="F87" t="s">
-        <v>7</v>
-      </c>
-      <c r="G87">
-        <v>31837</v>
-      </c>
-      <c r="H87">
-        <v>404169</v>
-      </c>
-      <c r="I87" s="2">
-        <v>142.29</v>
-      </c>
-      <c r="J87">
-        <v>190</v>
-      </c>
-      <c r="K87" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D88">
-        <v>1848</v>
-      </c>
-      <c r="E88">
-        <v>23772763</v>
-      </c>
-      <c r="F88" t="s">
-        <v>7</v>
-      </c>
-      <c r="G88">
-        <v>31703</v>
-      </c>
-      <c r="H88">
-        <v>46987</v>
-      </c>
-      <c r="I88" s="2">
-        <v>145.16999999999999</v>
-      </c>
-      <c r="J88">
-        <v>190</v>
-      </c>
-      <c r="K88" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G89" s="5" t="s">
+      <c r="N88">
+        <v>190</v>
+      </c>
+      <c r="O88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K89" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H89" s="4">
-        <f>SUM(H72:H88)/10000</f>
+      <c r="L89" s="4">
+        <f>SUM(L72:L88)/10000</f>
         <v>161.80410000000001</v>
       </c>
-      <c r="I89" s="2">
-        <f>SUMPRODUCT(H72:H88,I72:I88)/(H89*10000)</f>
+      <c r="M89" s="2">
+        <f>SUMPRODUCT(L72:L88,M72:M88)/(L89*10000)</f>
         <v>143.11835277968854</v>
       </c>
-      <c r="J89" t="s">
+      <c r="N89" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>16</v>
       </c>
@@ -3859,146 +3912,146 @@
       <c r="E91">
         <v>23772765</v>
       </c>
-      <c r="F91" t="s">
-        <v>7</v>
-      </c>
-      <c r="G91">
+      <c r="J91" t="s">
+        <v>7</v>
+      </c>
+      <c r="K91">
         <v>31765</v>
       </c>
-      <c r="H91">
+      <c r="L91">
         <v>24553</v>
       </c>
-      <c r="I91" s="2">
+      <c r="M91" s="2">
         <v>148.16999999999999</v>
       </c>
-      <c r="J91">
-        <v>190</v>
-      </c>
-      <c r="K91" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N91">
+        <v>190</v>
+      </c>
+      <c r="O91" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D92">
         <v>1881</v>
       </c>
       <c r="E92">
         <v>23774369</v>
       </c>
-      <c r="F92" t="s">
+      <c r="J92" t="s">
         <v>21</v>
       </c>
-      <c r="G92">
+      <c r="K92">
         <v>32211</v>
       </c>
-      <c r="H92">
+      <c r="L92">
         <v>87211</v>
       </c>
-      <c r="I92" s="2">
+      <c r="M92" s="2">
         <v>149.16</v>
       </c>
-      <c r="J92">
-        <v>190</v>
-      </c>
-      <c r="K92" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N92">
+        <v>190</v>
+      </c>
+      <c r="O92" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D93">
         <v>1777</v>
       </c>
       <c r="E93">
         <v>23772765</v>
       </c>
-      <c r="F93" t="s">
-        <v>7</v>
-      </c>
-      <c r="G93">
+      <c r="J93" t="s">
+        <v>7</v>
+      </c>
+      <c r="K93">
         <v>31801</v>
       </c>
-      <c r="H93">
+      <c r="L93">
         <v>33230</v>
       </c>
-      <c r="I93" s="2">
+      <c r="M93" s="2">
         <v>150.56</v>
       </c>
-      <c r="J93">
-        <v>190</v>
-      </c>
-      <c r="K93" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N93">
+        <v>190</v>
+      </c>
+      <c r="O93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D94">
         <v>1777</v>
       </c>
       <c r="E94">
         <v>23772765</v>
       </c>
-      <c r="F94" t="s">
-        <v>7</v>
-      </c>
-      <c r="G94">
+      <c r="J94" t="s">
+        <v>7</v>
+      </c>
+      <c r="K94">
         <v>31763</v>
       </c>
-      <c r="H94">
+      <c r="L94">
         <v>33344</v>
       </c>
-      <c r="I94" s="2">
+      <c r="M94" s="2">
         <v>149.97</v>
       </c>
-      <c r="J94">
-        <v>190</v>
-      </c>
-      <c r="K94" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N94">
+        <v>190</v>
+      </c>
+      <c r="O94" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D95">
         <v>1777</v>
       </c>
       <c r="E95">
         <v>23772765</v>
       </c>
-      <c r="F95" t="s">
-        <v>7</v>
-      </c>
-      <c r="G95">
+      <c r="J95" t="s">
+        <v>7</v>
+      </c>
+      <c r="K95">
         <v>31705</v>
       </c>
-      <c r="H95">
+      <c r="L95">
         <v>22260</v>
       </c>
-      <c r="I95" s="2">
+      <c r="M95" s="2">
         <v>149.04</v>
       </c>
-      <c r="J95">
-        <v>190</v>
-      </c>
-      <c r="K95" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G96" s="5" t="s">
+      <c r="N95">
+        <v>190</v>
+      </c>
+      <c r="O95" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K96" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H96" s="4">
-        <f>SUM(H91:H95)/10000</f>
+      <c r="L96" s="4">
+        <f>SUM(L91:L95)/10000</f>
         <v>20.059799999999999</v>
       </c>
-      <c r="I96" s="2">
-        <f>SUMPRODUCT(H91:H95,I91:I95)/(H96*10000)</f>
+      <c r="M96" s="2">
+        <f>SUMPRODUCT(L91:L95,M91:M95)/(L96*10000)</f>
         <v>149.39206597274151</v>
       </c>
-      <c r="J96" t="s">
+      <c r="N96" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>17</v>
       </c>
@@ -4014,46 +4067,46 @@
       <c r="E98">
         <v>23774413</v>
       </c>
-      <c r="F98" t="s">
+      <c r="J98" t="s">
         <v>21</v>
       </c>
-      <c r="G98">
+      <c r="K98">
         <v>31325</v>
       </c>
-      <c r="H98">
+      <c r="L98">
         <v>78961</v>
       </c>
-      <c r="I98" s="2">
+      <c r="M98" s="2">
         <v>161.96</v>
       </c>
-      <c r="J98">
-        <v>190</v>
-      </c>
-      <c r="K98" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G99" s="5" t="s">
+      <c r="N98">
+        <v>190</v>
+      </c>
+      <c r="O98" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K99" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H99" s="4">
-        <f>SUM(H98:H98)/10000</f>
+      <c r="L99" s="4">
+        <f>SUM(L98:L98)/10000</f>
         <v>7.8960999999999997</v>
       </c>
-      <c r="I99" s="2">
-        <f>SUMPRODUCT(H98:H98,I98:I98)/(H99*10000)</f>
+      <c r="M99" s="2">
+        <f>SUMPRODUCT(L98:L98,M98:M98)/(L99*10000)</f>
         <v>161.96</v>
       </c>
-      <c r="J99" t="s">
+      <c r="N99" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G100" s="5"/>
-      <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K100" s="5"/>
+      <c r="L100" s="4"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>18</v>
       </c>
@@ -4069,55 +4122,55 @@
       <c r="E101">
         <v>23773619</v>
       </c>
-      <c r="F101" t="s">
+      <c r="J101" t="s">
         <v>22</v>
       </c>
-      <c r="G101">
+      <c r="K101">
         <v>40260</v>
       </c>
-      <c r="H101">
+      <c r="L101">
         <v>412877</v>
       </c>
-      <c r="I101" s="2">
+      <c r="M101" s="2">
         <v>538.92999999999995</v>
       </c>
-      <c r="J101">
-        <v>190</v>
-      </c>
-      <c r="K101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G102" s="5" t="s">
+      <c r="N101">
+        <v>190</v>
+      </c>
+      <c r="O101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K102" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H102" s="4">
-        <f>SUM(H101:H101)/10000</f>
+      <c r="L102" s="4">
+        <f>SUM(L101:L101)/10000</f>
         <v>41.287700000000001</v>
       </c>
-      <c r="I102" s="2">
-        <f>SUMPRODUCT(H101:H101,I101:I101)/(H102*10000)</f>
+      <c r="M102" s="2">
+        <f>SUMPRODUCT(L101:L101,M101:M101)/(L102*10000)</f>
         <v>538.92999999999995</v>
       </c>
-      <c r="J102" t="s">
+      <c r="N102" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B103">
         <f>SUM(B2:B102)</f>
         <v>65</v>
       </c>
-      <c r="G103" s="5"/>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K103" s="5"/>
+      <c r="L103" s="4"/>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105">
         <f>WETL_ID!A23</f>
         <v>19</v>
@@ -4137,32 +4190,32 @@
         <f>WETL_ID!E23</f>
         <v>23809000</v>
       </c>
-      <c r="F105" t="str">
+      <c r="J105" t="str">
         <f>WETL_ID!F23</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G105">
+      <c r="K105">
         <f>WETL_ID!B23</f>
         <v>149851</v>
       </c>
-      <c r="H105">
+      <c r="L105">
         <v>50633</v>
       </c>
-      <c r="I105" s="2">
+      <c r="M105" s="2">
         <f>WETL_ID!D23</f>
         <v>5.81</v>
       </c>
-      <c r="J105">
-        <v>190</v>
-      </c>
-      <c r="K105" t="s">
-        <v>27</v>
-      </c>
-      <c r="L105" t="s">
+      <c r="N105">
+        <v>190</v>
+      </c>
+      <c r="O105" t="s">
+        <v>27</v>
+      </c>
+      <c r="P105" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107">
         <f>WETL_ID!A24</f>
         <v>20</v>
@@ -4182,29 +4235,29 @@
         <f>WETL_ID!E24</f>
         <v>23809000</v>
       </c>
-      <c r="F107" t="str">
+      <c r="J107" t="str">
         <f>WETL_ID!F24</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G107">
+      <c r="K107">
         <f>WETL_ID!B24</f>
         <v>150311</v>
       </c>
-      <c r="H107">
+      <c r="L107">
         <v>30651</v>
       </c>
-      <c r="I107" s="2">
+      <c r="M107" s="2">
         <f>WETL_ID!D24</f>
         <v>9.2799999999999994</v>
       </c>
-      <c r="J107">
-        <v>190</v>
-      </c>
-      <c r="K107" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N107">
+        <v>190</v>
+      </c>
+      <c r="O107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D108">
         <v>8121</v>
       </c>
@@ -4212,27 +4265,27 @@
         <f>WETL_ID!E25</f>
         <v>23809012</v>
       </c>
-      <c r="F108" t="str">
+      <c r="J108" t="str">
         <f>WETL_ID!F25</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G108">
+      <c r="K108">
         <v>150532</v>
       </c>
-      <c r="H108">
+      <c r="L108">
         <v>115205</v>
       </c>
-      <c r="I108" s="2">
+      <c r="M108" s="2">
         <v>12.75</v>
       </c>
-      <c r="J108">
-        <v>190</v>
-      </c>
-      <c r="K108" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N108">
+        <v>190</v>
+      </c>
+      <c r="O108" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D109">
         <v>8121</v>
       </c>
@@ -4240,47 +4293,47 @@
         <f>WETL_ID!E26</f>
         <v>23809054</v>
       </c>
-      <c r="F109" t="str">
+      <c r="J109" t="str">
         <f>WETL_ID!F26</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G109">
+      <c r="K109">
         <v>150537</v>
       </c>
-      <c r="H109">
+      <c r="L109">
         <v>73350</v>
       </c>
-      <c r="I109" s="2">
+      <c r="M109" s="2">
         <v>11.84</v>
       </c>
-      <c r="J109">
-        <v>190</v>
-      </c>
-      <c r="K109" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G110" s="5" t="s">
+      <c r="N109">
+        <v>190</v>
+      </c>
+      <c r="O109" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K110" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H110" s="4">
-        <f>SUM(H107:H109)/10000</f>
+      <c r="L110" s="4">
+        <f>SUM(L107:L109)/10000</f>
         <v>21.9206</v>
       </c>
-      <c r="I110" s="2">
-        <f>SUMPRODUCT(H107:H109,I107:I109)/(H110*10000)</f>
+      <c r="M110" s="2">
+        <f>SUMPRODUCT(L107:L109,M107:M109)/(L110*10000)</f>
         <v>11.960297756448274</v>
       </c>
-      <c r="J110" t="s">
+      <c r="N110" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G111" s="5"/>
-      <c r="H111" s="4"/>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K111" s="5"/>
+      <c r="L111" s="4"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112">
         <f>WETL_ID!A25</f>
         <v>21</v>
@@ -4300,55 +4353,55 @@
         <f>WETL_ID!E25</f>
         <v>23809012</v>
       </c>
-      <c r="F112" t="str">
+      <c r="J112" t="str">
         <f>WETL_ID!F25</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G112">
+      <c r="K112">
         <f>WETL_ID!B25</f>
         <v>151931</v>
       </c>
-      <c r="H112">
+      <c r="L112">
         <v>114846</v>
       </c>
-      <c r="I112" s="2">
+      <c r="M112" s="2">
         <f>WETL_ID!D25</f>
         <v>24.45</v>
       </c>
-      <c r="J112">
-        <v>190</v>
-      </c>
-      <c r="K112" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N112">
+        <v>190</v>
+      </c>
+      <c r="O112" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D113">
         <v>8177</v>
       </c>
       <c r="E113">
         <v>23809010</v>
       </c>
-      <c r="F113" t="s">
+      <c r="J113" t="s">
         <v>29</v>
       </c>
-      <c r="G113">
+      <c r="K113">
         <v>151913</v>
       </c>
-      <c r="H113">
+      <c r="L113">
         <v>48461</v>
       </c>
-      <c r="I113" s="2">
+      <c r="M113" s="2">
         <v>24.8</v>
       </c>
-      <c r="J113">
-        <v>190</v>
-      </c>
-      <c r="K113" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N113">
+        <v>190</v>
+      </c>
+      <c r="O113" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D114">
         <v>8210</v>
       </c>
@@ -4356,27 +4409,27 @@
         <f>WETL_ID!E27</f>
         <v>23809054</v>
       </c>
-      <c r="F114" t="str">
+      <c r="J114" t="str">
         <f>WETL_ID!F27</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G114">
+      <c r="K114">
         <v>151868</v>
       </c>
-      <c r="H114">
+      <c r="L114">
         <v>36088</v>
       </c>
-      <c r="I114" s="2">
+      <c r="M114" s="2">
         <v>26.37</v>
       </c>
-      <c r="J114">
-        <v>190</v>
-      </c>
-      <c r="K114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N114">
+        <v>190</v>
+      </c>
+      <c r="O114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D115">
         <v>8210</v>
       </c>
@@ -4384,47 +4437,47 @@
         <f>WETL_ID!E28</f>
         <v>23809054</v>
       </c>
-      <c r="F115" t="str">
+      <c r="J115" t="str">
         <f>WETL_ID!F28</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G115">
+      <c r="K115">
         <v>151932</v>
       </c>
-      <c r="H115">
+      <c r="L115">
         <v>158531</v>
       </c>
-      <c r="I115" s="2">
+      <c r="M115" s="2">
         <v>34.33</v>
       </c>
-      <c r="J115">
-        <v>190</v>
-      </c>
-      <c r="K115" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G116" s="5" t="s">
+      <c r="N115">
+        <v>190</v>
+      </c>
+      <c r="O115" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K116" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H116" s="4">
-        <f>SUM(H112:H115)/10000</f>
+      <c r="L116" s="4">
+        <f>SUM(L112:L115)/10000</f>
         <v>35.7926</v>
       </c>
-      <c r="I116" s="2">
-        <f>SUMPRODUCT(H112:H115,I112:I115)/(H116*10000)</f>
+      <c r="M116" s="2">
+        <f>SUMPRODUCT(L112:L115,M112:M115)/(L116*10000)</f>
         <v>29.066978341891897</v>
       </c>
-      <c r="J116" t="s">
+      <c r="N116" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G117" s="5"/>
-      <c r="H117" s="4"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K117" s="5"/>
+      <c r="L117" s="4"/>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118">
         <f>WETL_ID!A26</f>
         <v>22</v>
@@ -4444,29 +4497,29 @@
         <f>WETL_ID!E26</f>
         <v>23809054</v>
       </c>
-      <c r="F118" t="str">
+      <c r="J118" t="str">
         <f>WETL_ID!F26</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G118">
+      <c r="K118">
         <f>WETL_ID!B26</f>
         <v>150784</v>
       </c>
-      <c r="H118">
+      <c r="L118">
         <v>156359</v>
       </c>
-      <c r="I118" s="2">
+      <c r="M118" s="2">
         <f>WETL_ID!D26</f>
         <v>49.54</v>
       </c>
-      <c r="J118">
-        <v>190</v>
-      </c>
-      <c r="K118" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N118">
+        <v>190</v>
+      </c>
+      <c r="O118" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D119">
         <v>8048</v>
       </c>
@@ -4474,47 +4527,47 @@
         <f>WETL_ID!E27</f>
         <v>23809054</v>
       </c>
-      <c r="F119" t="str">
+      <c r="J119" t="str">
         <f>WETL_ID!F27</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G119">
+      <c r="K119">
         <v>150597</v>
       </c>
-      <c r="H119">
+      <c r="L119">
         <v>129261</v>
       </c>
-      <c r="I119" s="2">
+      <c r="M119" s="2">
         <v>49.96</v>
       </c>
-      <c r="J119">
-        <v>190</v>
-      </c>
-      <c r="K119" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G120" s="5" t="s">
+      <c r="N119">
+        <v>190</v>
+      </c>
+      <c r="O119" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K120" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H120" s="4">
-        <f>SUM(H118:H119)/10000</f>
+      <c r="L120" s="4">
+        <f>SUM(L118:L119)/10000</f>
         <v>28.562000000000001</v>
       </c>
-      <c r="I120" s="2">
-        <f>SUMPRODUCT(H118:H119,I118:I119)/(H120*10000)</f>
+      <c r="M120" s="2">
+        <f>SUMPRODUCT(L118:L119,M118:M119)/(L120*10000)</f>
         <v>49.730076395210418</v>
       </c>
-      <c r="J120" t="s">
+      <c r="N120" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G121" s="5"/>
-      <c r="H121" s="4"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K121" s="5"/>
+      <c r="L121" s="4"/>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122">
         <f>WETL_ID!A27</f>
         <v>23</v>
@@ -4534,55 +4587,55 @@
         <f>WETL_ID!E27</f>
         <v>23809054</v>
       </c>
-      <c r="F122" t="str">
+      <c r="J122" t="str">
         <f>WETL_ID!F27</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G122">
+      <c r="K122">
         <f>WETL_ID!B27</f>
         <v>150309</v>
       </c>
-      <c r="H122">
+      <c r="L122">
         <v>82608</v>
       </c>
-      <c r="I122" s="2">
+      <c r="M122" s="2">
         <f>WETL_ID!D27</f>
         <v>51.41</v>
       </c>
-      <c r="J122">
-        <v>190</v>
-      </c>
-      <c r="K122" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N122">
+        <v>190</v>
+      </c>
+      <c r="O122" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D123">
         <v>8048</v>
       </c>
       <c r="E123">
         <v>23809054</v>
       </c>
-      <c r="F123" t="s">
+      <c r="J123" t="s">
         <v>29</v>
       </c>
-      <c r="G123">
+      <c r="K123">
         <v>150308</v>
       </c>
-      <c r="H123">
+      <c r="L123">
         <v>63243</v>
       </c>
-      <c r="I123" s="2">
+      <c r="M123" s="2">
         <v>53.65</v>
       </c>
-      <c r="J123">
-        <v>190</v>
-      </c>
-      <c r="K123" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N123">
+        <v>190</v>
+      </c>
+      <c r="O123" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D124">
         <v>8048</v>
       </c>
@@ -4590,47 +4643,47 @@
         <f>WETL_ID!E28</f>
         <v>23809054</v>
       </c>
-      <c r="F124" t="str">
+      <c r="J124" t="str">
         <f>WETL_ID!F28</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G124">
+      <c r="K124">
         <v>150374</v>
       </c>
-      <c r="H124">
+      <c r="L124">
         <v>111581</v>
       </c>
-      <c r="I124" s="2">
+      <c r="M124" s="2">
         <v>54.99</v>
       </c>
-      <c r="J124">
-        <v>190</v>
-      </c>
-      <c r="K124" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G125" s="5" t="s">
+      <c r="N124">
+        <v>190</v>
+      </c>
+      <c r="O124" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K125" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H125" s="4">
-        <f>SUM(H122:H124)/10000</f>
+      <c r="L125" s="4">
+        <f>SUM(L122:L124)/10000</f>
         <v>25.743200000000002</v>
       </c>
-      <c r="I125" s="2">
-        <f>SUMPRODUCT(H122:H124,I122:I124)/(H125*10000)</f>
+      <c r="M125" s="2">
+        <f>SUMPRODUCT(L122:L124,M122:M124)/(L125*10000)</f>
         <v>53.512008685788857</v>
       </c>
-      <c r="J125" t="s">
+      <c r="N125" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G126" s="5"/>
-      <c r="H126" s="4"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K126" s="5"/>
+      <c r="L126" s="4"/>
+    </row>
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127">
         <f>WETL_ID!A28</f>
         <v>24</v>
@@ -4650,81 +4703,81 @@
         <f>WETL_ID!E28</f>
         <v>23809054</v>
       </c>
-      <c r="F127" t="str">
+      <c r="J127" t="str">
         <f>WETL_ID!F28</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G127">
+      <c r="K127">
         <f>WETL_ID!B28</f>
         <v>150066</v>
       </c>
-      <c r="H127">
+      <c r="L127">
         <v>114536</v>
       </c>
-      <c r="I127" s="2">
+      <c r="M127" s="2">
         <f>WETL_ID!D28</f>
         <v>53.87</v>
       </c>
-      <c r="J127">
-        <v>190</v>
-      </c>
-      <c r="K127" t="s">
-        <v>27</v>
-      </c>
-      <c r="L127" t="s">
+      <c r="N127">
+        <v>190</v>
+      </c>
+      <c r="O127" t="s">
+        <v>27</v>
+      </c>
+      <c r="P127" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D128">
         <v>8032</v>
       </c>
       <c r="E128">
         <v>23809056</v>
       </c>
-      <c r="F128" t="s">
+      <c r="J128" t="s">
         <v>29</v>
       </c>
-      <c r="G128">
+      <c r="K128">
         <v>149886</v>
       </c>
-      <c r="H128">
+      <c r="L128">
         <v>31686</v>
       </c>
-      <c r="I128" s="2">
+      <c r="M128" s="2">
         <v>55.48</v>
       </c>
-      <c r="J128">
-        <v>190</v>
-      </c>
-      <c r="K128" t="s">
-        <v>27</v>
-      </c>
-      <c r="L128" t="s">
+      <c r="N128">
+        <v>190</v>
+      </c>
+      <c r="O128" t="s">
+        <v>27</v>
+      </c>
+      <c r="P128" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G129" s="5" t="s">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K129" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H129" s="4">
-        <f>SUM(H127:H128)/10000</f>
+      <c r="L129" s="4">
+        <f>SUM(L127:L128)/10000</f>
         <v>14.622199999999999</v>
       </c>
-      <c r="I129" s="2">
-        <f>SUMPRODUCT(H127:H128,I127:I128)/(H129*10000)</f>
+      <c r="M129" s="2">
+        <f>SUMPRODUCT(L127:L128,M127:M128)/(L129*10000)</f>
         <v>54.218883615324643</v>
       </c>
-      <c r="J129" t="s">
+      <c r="N129" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G130" s="5"/>
-      <c r="H130" s="4"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K130" s="5"/>
+      <c r="L130" s="4"/>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131">
         <f>WETL_ID!A29</f>
         <v>25</v>
@@ -4744,197 +4797,197 @@
         <f>WETL_ID!E29</f>
         <v>23809058</v>
       </c>
-      <c r="F131" t="str">
+      <c r="J131" t="str">
         <f>WETL_ID!F29</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G131">
+      <c r="K131">
         <f>WETL_ID!B29</f>
         <v>149542</v>
       </c>
-      <c r="H131">
+      <c r="L131">
         <v>56060</v>
       </c>
-      <c r="I131" s="2">
+      <c r="M131" s="2">
         <f>WETL_ID!D29</f>
         <v>56.61</v>
       </c>
-      <c r="J131">
-        <v>190</v>
-      </c>
-      <c r="K131" t="s">
-        <v>27</v>
-      </c>
-      <c r="L131" t="s">
+      <c r="N131">
+        <v>190</v>
+      </c>
+      <c r="O131" t="s">
+        <v>27</v>
+      </c>
+      <c r="P131" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D132">
         <v>8059</v>
       </c>
       <c r="E132">
         <v>23809058</v>
       </c>
-      <c r="F132" t="s">
+      <c r="J132" t="s">
         <v>29</v>
       </c>
-      <c r="G132">
+      <c r="K132">
         <v>149302</v>
       </c>
-      <c r="H132">
+      <c r="L132">
         <v>106965</v>
       </c>
-      <c r="I132" s="2">
+      <c r="M132" s="2">
         <v>58.03</v>
       </c>
-      <c r="J132">
-        <v>190</v>
-      </c>
-      <c r="K132" t="s">
-        <v>27</v>
-      </c>
-      <c r="L132" t="s">
+      <c r="N132">
+        <v>190</v>
+      </c>
+      <c r="O132" t="s">
+        <v>27</v>
+      </c>
+      <c r="P132" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D133">
         <v>8059</v>
       </c>
       <c r="E133">
         <v>23809058</v>
       </c>
-      <c r="F133" t="s">
+      <c r="J133" t="s">
         <v>29</v>
       </c>
-      <c r="G133">
+      <c r="K133">
         <v>149553</v>
       </c>
-      <c r="H133">
+      <c r="L133">
         <v>108892</v>
       </c>
-      <c r="I133" s="2">
+      <c r="M133" s="2">
         <v>57.66</v>
       </c>
-      <c r="J133">
-        <v>190</v>
-      </c>
-      <c r="K133" t="s">
-        <v>27</v>
-      </c>
-      <c r="L133" t="s">
+      <c r="N133">
+        <v>190</v>
+      </c>
+      <c r="O133" t="s">
+        <v>27</v>
+      </c>
+      <c r="P133" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D134">
         <v>8032</v>
       </c>
       <c r="E134">
         <v>23809056</v>
       </c>
-      <c r="F134" t="s">
+      <c r="J134" t="s">
         <v>29</v>
       </c>
-      <c r="G134">
+      <c r="K134">
         <v>149599</v>
       </c>
-      <c r="H134">
+      <c r="L134">
         <v>30277</v>
       </c>
-      <c r="I134" s="2">
+      <c r="M134" s="2">
         <v>56.36</v>
       </c>
-      <c r="J134">
-        <v>190</v>
-      </c>
-      <c r="K134" t="s">
-        <v>27</v>
-      </c>
-      <c r="L134" t="s">
+      <c r="N134">
+        <v>190</v>
+      </c>
+      <c r="O134" t="s">
+        <v>27</v>
+      </c>
+      <c r="P134" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D135">
         <v>8059</v>
       </c>
       <c r="E135">
         <v>23809058</v>
       </c>
-      <c r="F135" t="s">
+      <c r="J135" t="s">
         <v>29</v>
       </c>
-      <c r="G135">
+      <c r="K135">
         <v>149525</v>
       </c>
-      <c r="H135">
+      <c r="L135">
         <v>26723</v>
       </c>
-      <c r="I135" s="2">
+      <c r="M135" s="2">
         <v>60.11</v>
       </c>
-      <c r="J135">
-        <v>190</v>
-      </c>
-      <c r="K135" t="s">
-        <v>27</v>
-      </c>
-      <c r="L135" t="s">
+      <c r="N135">
+        <v>190</v>
+      </c>
+      <c r="O135" t="s">
+        <v>27</v>
+      </c>
+      <c r="P135" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D136">
         <v>8059</v>
       </c>
       <c r="E136">
         <v>23809058</v>
       </c>
-      <c r="F136" t="s">
+      <c r="J136" t="s">
         <v>29</v>
       </c>
-      <c r="G136">
+      <c r="K136">
         <v>149394</v>
       </c>
-      <c r="H136">
+      <c r="L136">
         <v>46447</v>
       </c>
-      <c r="I136" s="2">
+      <c r="M136" s="2">
         <v>56.94</v>
       </c>
-      <c r="J136">
-        <v>190</v>
-      </c>
-      <c r="K136" t="s">
-        <v>27</v>
-      </c>
-      <c r="L136" t="s">
+      <c r="N136">
+        <v>190</v>
+      </c>
+      <c r="O136" t="s">
+        <v>27</v>
+      </c>
+      <c r="P136" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G137" s="5" t="s">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K137" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H137" s="4">
-        <f>SUM(H131:H136)/10000</f>
+      <c r="L137" s="4">
+        <f>SUM(L131:L136)/10000</f>
         <v>37.5364</v>
       </c>
-      <c r="I137" s="2">
-        <f>SUMPRODUCT(H131:H136,I131:I136)/(H137*10000)</f>
+      <c r="M137" s="2">
+        <f>SUMPRODUCT(L131:L136,M131:M136)/(L137*10000)</f>
         <v>57.589091388625441</v>
       </c>
-      <c r="J137" t="s">
+      <c r="N137" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G138" s="5"/>
-      <c r="H138" s="4"/>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K138" s="5"/>
+      <c r="L138" s="4"/>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139">
         <f>WETL_ID!A30</f>
         <v>26</v>
@@ -4954,25 +5007,25 @@
         <f>WETL_ID!E30</f>
         <v>23815518</v>
       </c>
-      <c r="G139">
+      <c r="K139">
         <f>WETL_ID!B30</f>
         <v>153673</v>
       </c>
-      <c r="H139">
+      <c r="L139">
         <v>52785</v>
       </c>
-      <c r="I139" s="2">
+      <c r="M139" s="2">
         <f>WETL_ID!D30</f>
         <v>252.65</v>
       </c>
-      <c r="J139">
-        <v>190</v>
-      </c>
-      <c r="K139" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N139">
+        <v>190</v>
+      </c>
+      <c r="O139" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140">
         <f>WETL_ID!A31</f>
         <v>27</v>
@@ -4992,29 +5045,29 @@
         <f>WETL_ID!E31</f>
         <v>23815444</v>
       </c>
-      <c r="F140" t="str">
+      <c r="J140" t="str">
         <f>WETL_ID!F31</f>
         <v>Crystal Springs Cr</v>
       </c>
-      <c r="G140">
+      <c r="K140">
         <f>WETL_ID!B31</f>
         <v>156391</v>
       </c>
-      <c r="H140">
+      <c r="L140">
         <v>55853</v>
       </c>
-      <c r="I140" s="2">
+      <c r="M140" s="2">
         <f>WETL_ID!D31</f>
         <v>30.94</v>
       </c>
-      <c r="J140">
-        <v>190</v>
-      </c>
-      <c r="K140" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N140">
+        <v>190</v>
+      </c>
+      <c r="O140" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141">
         <f>WETL_ID!A32</f>
         <v>28</v>
@@ -5034,29 +5087,29 @@
         <f>WETL_ID!E32</f>
         <v>23815070</v>
       </c>
-      <c r="F141" t="str">
+      <c r="J141" t="str">
         <f>WETL_ID!F32</f>
         <v>Johnson Cr</v>
       </c>
-      <c r="G141">
+      <c r="K141">
         <f>WETL_ID!B32</f>
         <v>156910</v>
       </c>
-      <c r="H141">
+      <c r="L141">
         <v>67222</v>
       </c>
-      <c r="I141" s="2">
+      <c r="M141" s="2">
         <f>WETL_ID!D32</f>
         <v>95.08</v>
       </c>
-      <c r="J141">
-        <v>190</v>
-      </c>
-      <c r="K141" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N141">
+        <v>190</v>
+      </c>
+      <c r="O141" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142">
         <f>WETL_ID!A33</f>
         <v>29</v>
@@ -5076,32 +5129,32 @@
         <f>WETL_ID!E33</f>
         <v>23809078</v>
       </c>
-      <c r="F142" t="str">
+      <c r="J142" t="str">
         <f>WETL_ID!F33</f>
         <v>Clackamas R</v>
       </c>
-      <c r="G142">
+      <c r="K142">
         <f>WETL_ID!B33</f>
         <v>145278</v>
       </c>
-      <c r="H142">
+      <c r="L142">
         <v>102588</v>
       </c>
-      <c r="I142" s="2">
+      <c r="M142" s="2">
         <f>WETL_ID!D33</f>
         <v>86.9</v>
       </c>
-      <c r="J142">
-        <v>190</v>
-      </c>
-      <c r="K142" t="s">
-        <v>27</v>
-      </c>
-      <c r="L142" t="s">
+      <c r="N142">
+        <v>190</v>
+      </c>
+      <c r="O142" t="s">
+        <v>27</v>
+      </c>
+      <c r="P142" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143">
         <f>WETL_ID!A34</f>
         <v>30</v>
@@ -5121,32 +5174,35 @@
         <f>WETL_ID!E34</f>
         <v>23809418</v>
       </c>
-      <c r="F143" t="str">
+      <c r="J143" t="str">
         <f>WETL_ID!F34</f>
         <v>Oak Grove Fork Clackamas R</v>
       </c>
-      <c r="G143">
+      <c r="K143">
         <f>WETL_ID!B34</f>
         <v>120758</v>
       </c>
-      <c r="H143">
+      <c r="L143">
         <v>65830</v>
       </c>
-      <c r="I143" s="2">
+      <c r="M143" s="2">
         <f>WETL_ID!D34</f>
         <v>665.6</v>
       </c>
-      <c r="J143">
-        <v>190</v>
-      </c>
-      <c r="K143" t="s">
-        <v>27</v>
-      </c>
-      <c r="L143" t="s">
+      <c r="N143">
+        <v>190</v>
+      </c>
+      <c r="O143" t="s">
+        <v>27</v>
+      </c>
+      <c r="P143" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D72:O88">
+    <sortCondition ref="M72:M88"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Set up the No_wetlands_demo scenario. Reporter_McKenzie.xml - Add PRECIP_YR and TEMP_YR to the REP Wetland 15 report. SimulationScenarios.xml - Add the No_wetlands_demo scenario. APs.cpp - Fix a logic error in FindInIntCArray(), called by InitRunPrescribedLULCs(). Add a ScenarioData/No_wetlands_demo folder, cloned from the Baseline_Demo folder but with a different prescribedLULCS.csv file.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA848A8-73AA-4391-AA65-4D084AEC8F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5CB166-E70F-4E03-9300-C4F5F453C8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="52">
   <si>
     <t>WETL_ID</t>
   </si>
@@ -188,6 +188,9 @@
   <si>
     <t>reach also spills into wetl 15</t>
   </si>
+  <si>
+    <t>HRU 1909 is composed entirely of IDU 31796</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -239,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -263,6 +272,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1933,8 +1943,8 @@
   <dimension ref="A1:P143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3303,7 +3313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>13</v>
       </c>
@@ -3338,7 +3348,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K67" s="5" t="s">
         <v>20</v>
       </c>
@@ -3354,7 +3364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>14</v>
       </c>
@@ -3389,7 +3399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K70" s="5" t="s">
         <v>20</v>
       </c>
@@ -3405,7 +3415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D73">
         <v>1928</v>
       </c>
@@ -3480,7 +3490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D74">
         <v>1821</v>
       </c>
@@ -3506,7 +3516,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D75">
         <v>1941</v>
       </c>
@@ -3532,7 +3542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D76">
         <v>1939</v>
       </c>
@@ -3558,7 +3568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D77">
         <v>1821</v>
       </c>
@@ -3584,7 +3594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D78">
         <v>1821</v>
       </c>
@@ -3610,7 +3620,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D79">
         <v>1928</v>
       </c>
@@ -3636,8 +3646,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="D80">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D80" s="13">
         <v>1909</v>
       </c>
       <c r="E80">
@@ -3646,7 +3656,7 @@
       <c r="J80" t="s">
         <v>7</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="13">
         <v>31796</v>
       </c>
       <c r="L80">
@@ -3660,6 +3670,9 @@
       </c>
       <c r="O80" t="s">
         <v>27</v>
+      </c>
+      <c r="P80" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add energy and temperature terms to water balance log entries. ClimateScenarios.xml - Change a comment. Flow.cpp - Add energy and temperature terms to log message in EndYear(). WaterRights.cpp - Add energy and temperature terms to AltWaterMaster::Init(), InitRun(), StartYear(), and EndYear().
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BB4DB8-5356-4FCA-91E3-048ECD2D2F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC98C0A1-A85C-4F85-B3DE-70691774F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
   <sheets>
     <sheet name="WETL_ID" sheetId="1" r:id="rId1"/>
     <sheet name="IDUs" sheetId="2" r:id="rId2"/>
+    <sheet name="IDUs (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="56">
   <si>
     <t>WETL_ID</t>
   </si>
@@ -200,6 +201,9 @@
   <si>
     <t>Wetlands as in CW3M C705 11/19/21 in the McKenzie, Clackamas, and Nsantiam basins</t>
   </si>
+  <si>
+    <t># reaches</t>
+  </si>
 </sst>
 </file>
 
@@ -225,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -257,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,6 +292,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4153BDD9-3748-4423-B686-257FDC6E887B}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="13" topLeftCell="K26" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="10" ySplit="13" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
       <selection pane="bottomRight"/>
@@ -1995,8 +2007,8 @@
   <dimension ref="A1:P143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P80" sqref="P80"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2096,6 +2108,9 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="D4">
         <v>2274</v>
       </c>
@@ -2122,6 +2137,9 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="D5">
         <v>2251</v>
       </c>
@@ -2148,6 +2166,9 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
       <c r="D6">
         <v>2251</v>
       </c>
@@ -2174,6 +2195,9 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
       <c r="D7">
         <v>2250</v>
       </c>
@@ -2254,6 +2278,9 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
       <c r="D11">
         <v>2194</v>
       </c>
@@ -2331,6 +2358,9 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
       <c r="D15">
         <v>2198</v>
       </c>
@@ -2354,6 +2384,9 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
       <c r="D16">
         <v>2194</v>
       </c>
@@ -2380,6 +2413,9 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
       <c r="D17">
         <v>2206</v>
       </c>
@@ -2454,6 +2490,9 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
       <c r="D21">
         <v>2069</v>
       </c>
@@ -2534,6 +2573,9 @@
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
       <c r="D25">
         <v>2069</v>
       </c>
@@ -2563,6 +2605,9 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
       <c r="D26">
         <v>2069</v>
       </c>
@@ -2691,6 +2736,9 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>7</v>
+      </c>
       <c r="D33">
         <v>2122</v>
       </c>
@@ -2717,6 +2765,9 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
       <c r="D34">
         <v>2004</v>
       </c>
@@ -2740,6 +2791,9 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>7</v>
+      </c>
       <c r="D35">
         <v>2037</v>
       </c>
@@ -2766,6 +2820,9 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>7</v>
+      </c>
       <c r="D36">
         <v>2004</v>
       </c>
@@ -2888,6 +2945,9 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>9</v>
+      </c>
       <c r="D43">
         <v>2037</v>
       </c>
@@ -2914,6 +2974,9 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>9</v>
+      </c>
       <c r="D44">
         <v>2037</v>
       </c>
@@ -2991,6 +3054,9 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>10</v>
+      </c>
       <c r="D48">
         <v>2033</v>
       </c>
@@ -3068,6 +3134,9 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>11</v>
+      </c>
       <c r="D52">
         <v>2005</v>
       </c>
@@ -3094,6 +3163,9 @@
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>11</v>
+      </c>
       <c r="D53">
         <v>1966</v>
       </c>
@@ -3120,6 +3192,9 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>11</v>
+      </c>
       <c r="D54">
         <v>1966</v>
       </c>
@@ -3146,6 +3221,9 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>11</v>
+      </c>
       <c r="D55">
         <v>1966</v>
       </c>
@@ -3172,6 +3250,9 @@
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>11</v>
+      </c>
       <c r="D56">
         <v>2005</v>
       </c>
@@ -3249,6 +3330,9 @@
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>12</v>
+      </c>
       <c r="D60">
         <v>1972</v>
       </c>
@@ -3272,6 +3356,9 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>12</v>
+      </c>
       <c r="D61">
         <v>1946</v>
       </c>
@@ -3298,6 +3385,9 @@
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>12</v>
+      </c>
       <c r="D62">
         <v>1972</v>
       </c>
@@ -3324,6 +3414,9 @@
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>12</v>
+      </c>
       <c r="D63">
         <v>1946</v>
       </c>
@@ -3517,6 +3610,9 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>15</v>
+      </c>
       <c r="D73">
         <v>1928</v>
       </c>
@@ -3543,6 +3639,9 @@
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>15</v>
+      </c>
       <c r="D74">
         <v>1821</v>
       </c>
@@ -3569,6 +3668,9 @@
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>15</v>
+      </c>
       <c r="D75">
         <v>1941</v>
       </c>
@@ -3595,6 +3697,9 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>15</v>
+      </c>
       <c r="D76">
         <v>1939</v>
       </c>
@@ -3621,6 +3726,9 @@
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>15</v>
+      </c>
       <c r="D77">
         <v>1821</v>
       </c>
@@ -3647,6 +3755,9 @@
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>15</v>
+      </c>
       <c r="D78">
         <v>1821</v>
       </c>
@@ -3673,6 +3784,9 @@
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>15</v>
+      </c>
       <c r="D79">
         <v>1928</v>
       </c>
@@ -3699,6 +3813,9 @@
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>15</v>
+      </c>
       <c r="D80" s="13">
         <v>1909</v>
       </c>
@@ -3728,6 +3845,9 @@
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>15</v>
+      </c>
       <c r="D81">
         <v>1939</v>
       </c>
@@ -3754,6 +3874,9 @@
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>15</v>
+      </c>
       <c r="D82">
         <v>1928</v>
       </c>
@@ -3780,6 +3903,9 @@
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>15</v>
+      </c>
       <c r="D83">
         <v>1848</v>
       </c>
@@ -3806,6 +3932,9 @@
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>15</v>
+      </c>
       <c r="D84">
         <v>1928</v>
       </c>
@@ -3832,6 +3961,9 @@
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>15</v>
+      </c>
       <c r="D85">
         <v>1928</v>
       </c>
@@ -3858,6 +3990,9 @@
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>15</v>
+      </c>
       <c r="D86">
         <v>1848</v>
       </c>
@@ -3884,6 +4019,9 @@
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>15</v>
+      </c>
       <c r="D87">
         <v>1777</v>
       </c>
@@ -3910,6 +4048,9 @@
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>15</v>
+      </c>
       <c r="D88">
         <v>1928</v>
       </c>
@@ -4004,6 +4145,9 @@
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>16</v>
+      </c>
       <c r="D92">
         <v>1881</v>
       </c>
@@ -4030,6 +4174,9 @@
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>16</v>
+      </c>
       <c r="D93">
         <v>1777</v>
       </c>
@@ -4056,6 +4203,9 @@
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>16</v>
+      </c>
       <c r="D94">
         <v>1777</v>
       </c>
@@ -4082,6 +4232,9 @@
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>16</v>
+      </c>
       <c r="D95">
         <v>1777</v>
       </c>
@@ -5278,4 +5431,3497 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9225645-945C-4C81-90D4-9241866A6700}">
+  <dimension ref="A1:Q143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
+        <v>5</v>
+      </c>
+      <c r="D2" s="14">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14">
+        <v>2277</v>
+      </c>
+      <c r="F2" s="14">
+        <v>23765583</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="14">
+        <v>37310</v>
+      </c>
+      <c r="M2" s="14">
+        <v>44172</v>
+      </c>
+      <c r="N2" s="15">
+        <v>113.24</v>
+      </c>
+      <c r="O2" s="14">
+        <v>190</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2274</v>
+      </c>
+      <c r="F3">
+        <v>23772703</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>37279</v>
+      </c>
+      <c r="M3">
+        <v>97565</v>
+      </c>
+      <c r="N3" s="2">
+        <v>114.32</v>
+      </c>
+      <c r="O3">
+        <v>190</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2251</v>
+      </c>
+      <c r="F4">
+        <v>23772705</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4">
+        <v>36873</v>
+      </c>
+      <c r="M4">
+        <v>30567</v>
+      </c>
+      <c r="N4" s="2">
+        <v>115.07</v>
+      </c>
+      <c r="O4">
+        <v>190</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2251</v>
+      </c>
+      <c r="F5">
+        <v>23772705</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>37240</v>
+      </c>
+      <c r="M5">
+        <v>23708</v>
+      </c>
+      <c r="N5" s="2">
+        <v>115.86</v>
+      </c>
+      <c r="O5">
+        <v>195</v>
+      </c>
+      <c r="P5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2250</v>
+      </c>
+      <c r="F6">
+        <v>23772713</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>36850</v>
+      </c>
+      <c r="M6">
+        <v>45045</v>
+      </c>
+      <c r="N6" s="2">
+        <v>116.67</v>
+      </c>
+      <c r="O6">
+        <v>195</v>
+      </c>
+      <c r="P6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2</v>
+      </c>
+      <c r="D7" s="14">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14">
+        <v>2244</v>
+      </c>
+      <c r="F7" s="14">
+        <v>23772709</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="14">
+        <v>36786</v>
+      </c>
+      <c r="M7" s="14">
+        <v>71657</v>
+      </c>
+      <c r="N7" s="15">
+        <v>115.72</v>
+      </c>
+      <c r="O7" s="14">
+        <v>195</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2194</v>
+      </c>
+      <c r="F8">
+        <v>23772709</v>
+      </c>
+      <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>36776</v>
+      </c>
+      <c r="M8">
+        <v>56719</v>
+      </c>
+      <c r="N8" s="2">
+        <v>116.08</v>
+      </c>
+      <c r="O8">
+        <v>195</v>
+      </c>
+      <c r="P8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>4</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14">
+        <v>2194</v>
+      </c>
+      <c r="F9" s="14">
+        <v>23772717</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="14">
+        <v>36282</v>
+      </c>
+      <c r="M9" s="14">
+        <v>32023</v>
+      </c>
+      <c r="N9" s="15">
+        <v>118.28</v>
+      </c>
+      <c r="O9" s="14">
+        <v>190</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>2209</v>
+      </c>
+      <c r="F10">
+        <v>23772721</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <v>36356</v>
+      </c>
+      <c r="M10">
+        <v>39502</v>
+      </c>
+      <c r="N10" s="2">
+        <v>117.98</v>
+      </c>
+      <c r="O10">
+        <v>190</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>2206</v>
+      </c>
+      <c r="F11">
+        <v>23774111</v>
+      </c>
+      <c r="L11">
+        <v>36345</v>
+      </c>
+      <c r="M11">
+        <v>42644</v>
+      </c>
+      <c r="N11" s="2">
+        <v>118.42</v>
+      </c>
+      <c r="O11">
+        <v>190</v>
+      </c>
+      <c r="P11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>2198</v>
+      </c>
+      <c r="F12">
+        <v>23774113</v>
+      </c>
+      <c r="L12">
+        <v>36324</v>
+      </c>
+      <c r="M12">
+        <v>81228</v>
+      </c>
+      <c r="N12" s="2">
+        <v>117.67</v>
+      </c>
+      <c r="O12">
+        <v>190</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="14">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13" s="14">
+        <v>2</v>
+      </c>
+      <c r="E13" s="14">
+        <v>2170</v>
+      </c>
+      <c r="F13" s="14">
+        <v>23772725</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="14">
+        <v>36305</v>
+      </c>
+      <c r="M13" s="14">
+        <v>30363</v>
+      </c>
+      <c r="N13" s="15">
+        <v>119.5</v>
+      </c>
+      <c r="O13" s="14">
+        <v>190</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>2069</v>
+      </c>
+      <c r="F14">
+        <v>23772727</v>
+      </c>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <v>36307</v>
+      </c>
+      <c r="M14">
+        <v>116500</v>
+      </c>
+      <c r="N14" s="2">
+        <v>120.72</v>
+      </c>
+      <c r="O14">
+        <v>190</v>
+      </c>
+      <c r="P14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>1</v>
+      </c>
+      <c r="B15" s="14">
+        <v>5</v>
+      </c>
+      <c r="C15" s="14">
+        <v>3</v>
+      </c>
+      <c r="D15" s="14">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14">
+        <v>2069</v>
+      </c>
+      <c r="F15" s="14">
+        <v>23772727</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="14">
+        <v>36255</v>
+      </c>
+      <c r="M15" s="14">
+        <v>250687</v>
+      </c>
+      <c r="N15" s="15">
+        <v>124.08</v>
+      </c>
+      <c r="O15" s="14">
+        <v>190</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>2069</v>
+      </c>
+      <c r="F16">
+        <v>23772727</v>
+      </c>
+      <c r="K16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <v>36228</v>
+      </c>
+      <c r="M16">
+        <v>36958</v>
+      </c>
+      <c r="N16" s="2">
+        <v>123.13</v>
+      </c>
+      <c r="O16">
+        <v>190</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>2069</v>
+      </c>
+      <c r="F17">
+        <v>23772727</v>
+      </c>
+      <c r="K17" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>36220</v>
+      </c>
+      <c r="M17">
+        <v>64343</v>
+      </c>
+      <c r="N17" s="2">
+        <v>124.78</v>
+      </c>
+      <c r="O17">
+        <v>190</v>
+      </c>
+      <c r="P17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>1</v>
+      </c>
+      <c r="B18" s="14">
+        <v>6</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1</v>
+      </c>
+      <c r="E18" s="14">
+        <v>2069</v>
+      </c>
+      <c r="F18" s="14">
+        <v>23772727</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="14">
+        <v>35846</v>
+      </c>
+      <c r="M18" s="14">
+        <v>141017</v>
+      </c>
+      <c r="N18" s="15">
+        <v>122.91</v>
+      </c>
+      <c r="O18" s="14">
+        <v>190</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>4</v>
+      </c>
+      <c r="B19" s="14">
+        <v>7</v>
+      </c>
+      <c r="C19" s="14">
+        <v>5</v>
+      </c>
+      <c r="D19" s="14">
+        <v>4</v>
+      </c>
+      <c r="E19" s="14">
+        <v>2069</v>
+      </c>
+      <c r="F19" s="14">
+        <v>23772727</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="14">
+        <v>35767</v>
+      </c>
+      <c r="M19" s="14">
+        <v>137221</v>
+      </c>
+      <c r="N19" s="15">
+        <v>123.88</v>
+      </c>
+      <c r="O19" s="14">
+        <v>190</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>2122</v>
+      </c>
+      <c r="F20">
+        <v>23772729</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <v>35332</v>
+      </c>
+      <c r="M20">
+        <v>75379</v>
+      </c>
+      <c r="N20" s="2">
+        <v>126.88</v>
+      </c>
+      <c r="O20">
+        <v>190</v>
+      </c>
+      <c r="P20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>2037</v>
+      </c>
+      <c r="F21">
+        <v>23772731</v>
+      </c>
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>35243</v>
+      </c>
+      <c r="M21">
+        <v>44085</v>
+      </c>
+      <c r="N21" s="2">
+        <v>125.35</v>
+      </c>
+      <c r="O21">
+        <v>190</v>
+      </c>
+      <c r="P21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>2004</v>
+      </c>
+      <c r="F22">
+        <v>23774181</v>
+      </c>
+      <c r="L22">
+        <v>35244</v>
+      </c>
+      <c r="M22">
+        <v>28533</v>
+      </c>
+      <c r="N22" s="2">
+        <v>127.06</v>
+      </c>
+      <c r="O22">
+        <v>190</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>2004</v>
+      </c>
+      <c r="F23">
+        <v>23774181</v>
+      </c>
+      <c r="L23">
+        <v>35233</v>
+      </c>
+      <c r="M23">
+        <v>45898</v>
+      </c>
+      <c r="N23" s="2">
+        <v>126.24</v>
+      </c>
+      <c r="O23">
+        <v>190</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>1</v>
+      </c>
+      <c r="B24" s="14">
+        <v>8</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1</v>
+      </c>
+      <c r="E24" s="14">
+        <v>2004</v>
+      </c>
+      <c r="F24" s="14">
+        <v>23774181</v>
+      </c>
+      <c r="L24" s="14">
+        <v>34761</v>
+      </c>
+      <c r="M24" s="14">
+        <v>104520</v>
+      </c>
+      <c r="N24" s="15">
+        <v>128.61000000000001</v>
+      </c>
+      <c r="O24" s="14">
+        <v>190</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>1</v>
+      </c>
+      <c r="B25" s="14">
+        <v>9</v>
+      </c>
+      <c r="C25" s="14">
+        <v>3</v>
+      </c>
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="14">
+        <v>2037</v>
+      </c>
+      <c r="F25" s="14">
+        <v>23772731</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="14">
+        <v>34773</v>
+      </c>
+      <c r="M25" s="14">
+        <v>149305</v>
+      </c>
+      <c r="N25" s="15">
+        <v>128.71</v>
+      </c>
+      <c r="O25" s="14">
+        <v>190</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>2037</v>
+      </c>
+      <c r="F26">
+        <v>23772731</v>
+      </c>
+      <c r="K26" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>34764</v>
+      </c>
+      <c r="M26">
+        <v>134530</v>
+      </c>
+      <c r="N26" s="2">
+        <v>128.31</v>
+      </c>
+      <c r="O26">
+        <v>190</v>
+      </c>
+      <c r="P26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>2037</v>
+      </c>
+      <c r="F27">
+        <v>23772731</v>
+      </c>
+      <c r="K27" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27">
+        <v>34344</v>
+      </c>
+      <c r="M27">
+        <v>24108</v>
+      </c>
+      <c r="N27" s="2">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="O27">
+        <v>190</v>
+      </c>
+      <c r="P27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>1</v>
+      </c>
+      <c r="B28" s="14">
+        <v>10</v>
+      </c>
+      <c r="C28" s="14">
+        <v>2</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="14">
+        <v>2033</v>
+      </c>
+      <c r="F28" s="14">
+        <v>23772737</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="14">
+        <v>33827</v>
+      </c>
+      <c r="M28" s="14">
+        <v>41473</v>
+      </c>
+      <c r="N28" s="15">
+        <v>132.80000000000001</v>
+      </c>
+      <c r="O28" s="14">
+        <v>190</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>2033</v>
+      </c>
+      <c r="F29">
+        <v>23772737</v>
+      </c>
+      <c r="K29" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29">
+        <v>33807</v>
+      </c>
+      <c r="M29">
+        <v>43240</v>
+      </c>
+      <c r="N29" s="2">
+        <v>130.38</v>
+      </c>
+      <c r="O29">
+        <v>190</v>
+      </c>
+      <c r="P29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>2</v>
+      </c>
+      <c r="B30" s="14">
+        <v>11</v>
+      </c>
+      <c r="C30" s="14">
+        <v>6</v>
+      </c>
+      <c r="D30" s="14">
+        <v>2</v>
+      </c>
+      <c r="E30" s="14">
+        <v>2005</v>
+      </c>
+      <c r="F30" s="14">
+        <v>23772739</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" s="14">
+        <v>33362</v>
+      </c>
+      <c r="M30" s="14">
+        <v>41477</v>
+      </c>
+      <c r="N30" s="15">
+        <v>129.62</v>
+      </c>
+      <c r="O30" s="14">
+        <v>190</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="E31">
+        <v>2005</v>
+      </c>
+      <c r="F31">
+        <v>23772739</v>
+      </c>
+      <c r="K31" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31">
+        <v>33323</v>
+      </c>
+      <c r="M31">
+        <v>54647</v>
+      </c>
+      <c r="N31" s="2">
+        <v>130.16</v>
+      </c>
+      <c r="O31">
+        <v>190</v>
+      </c>
+      <c r="P31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>2005</v>
+      </c>
+      <c r="F32">
+        <v>23772739</v>
+      </c>
+      <c r="K32" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32">
+        <v>33724</v>
+      </c>
+      <c r="M32">
+        <v>28116</v>
+      </c>
+      <c r="N32" s="2">
+        <v>132.88999999999999</v>
+      </c>
+      <c r="O32">
+        <v>190</v>
+      </c>
+      <c r="P32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <v>1966</v>
+      </c>
+      <c r="F33">
+        <v>23772741</v>
+      </c>
+      <c r="K33" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33">
+        <v>33303</v>
+      </c>
+      <c r="M33">
+        <v>33230</v>
+      </c>
+      <c r="N33" s="2">
+        <v>130.08000000000001</v>
+      </c>
+      <c r="O33">
+        <v>190</v>
+      </c>
+      <c r="P33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="E34">
+        <v>1966</v>
+      </c>
+      <c r="F34">
+        <v>23772741</v>
+      </c>
+      <c r="K34" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34">
+        <v>33310</v>
+      </c>
+      <c r="M34">
+        <v>149289</v>
+      </c>
+      <c r="N34" s="2">
+        <v>130.51</v>
+      </c>
+      <c r="O34">
+        <v>190</v>
+      </c>
+      <c r="P34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>1966</v>
+      </c>
+      <c r="F35">
+        <v>23772741</v>
+      </c>
+      <c r="K35" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35">
+        <v>33349</v>
+      </c>
+      <c r="M35">
+        <v>59644</v>
+      </c>
+      <c r="N35" s="2">
+        <v>131.46</v>
+      </c>
+      <c r="O35">
+        <v>190</v>
+      </c>
+      <c r="P35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>3</v>
+      </c>
+      <c r="B36" s="14">
+        <v>12</v>
+      </c>
+      <c r="C36" s="14">
+        <v>5</v>
+      </c>
+      <c r="D36" s="14">
+        <v>2</v>
+      </c>
+      <c r="E36" s="14">
+        <v>1945</v>
+      </c>
+      <c r="F36" s="14">
+        <v>23772743</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="14">
+        <v>32813</v>
+      </c>
+      <c r="M36" s="14">
+        <v>23559</v>
+      </c>
+      <c r="N36" s="15">
+        <v>135</v>
+      </c>
+      <c r="O36" s="14">
+        <v>190</v>
+      </c>
+      <c r="P36" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="E37">
+        <v>1946</v>
+      </c>
+      <c r="F37">
+        <v>23772745</v>
+      </c>
+      <c r="K37" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37">
+        <v>33278</v>
+      </c>
+      <c r="M37">
+        <v>80665</v>
+      </c>
+      <c r="N37" s="2">
+        <v>133.43</v>
+      </c>
+      <c r="O37">
+        <v>190</v>
+      </c>
+      <c r="P37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>1946</v>
+      </c>
+      <c r="F38">
+        <v>23772745</v>
+      </c>
+      <c r="K38" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <v>33324</v>
+      </c>
+      <c r="M38">
+        <v>82089</v>
+      </c>
+      <c r="N38" s="2">
+        <v>134.77000000000001</v>
+      </c>
+      <c r="O38">
+        <v>190</v>
+      </c>
+      <c r="P38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="E39">
+        <v>1972</v>
+      </c>
+      <c r="F39">
+        <v>23774285</v>
+      </c>
+      <c r="L39">
+        <v>32865</v>
+      </c>
+      <c r="M39">
+        <v>53187</v>
+      </c>
+      <c r="N39" s="2">
+        <v>134.47999999999999</v>
+      </c>
+      <c r="O39">
+        <v>190</v>
+      </c>
+      <c r="P39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>1972</v>
+      </c>
+      <c r="F40">
+        <v>23774285</v>
+      </c>
+      <c r="L40">
+        <v>33262</v>
+      </c>
+      <c r="M40">
+        <v>23268</v>
+      </c>
+      <c r="N40" s="3">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>190</v>
+      </c>
+      <c r="P40" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
+        <v>1</v>
+      </c>
+      <c r="B41" s="14">
+        <v>13</v>
+      </c>
+      <c r="C41" s="14">
+        <v>1</v>
+      </c>
+      <c r="D41" s="14">
+        <v>1</v>
+      </c>
+      <c r="E41" s="14">
+        <v>1946</v>
+      </c>
+      <c r="F41" s="14">
+        <v>23772745</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L41" s="14">
+        <v>33306</v>
+      </c>
+      <c r="M41" s="14">
+        <v>65332</v>
+      </c>
+      <c r="N41" s="15">
+        <v>134.74</v>
+      </c>
+      <c r="O41" s="14">
+        <v>190</v>
+      </c>
+      <c r="P41" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>1</v>
+      </c>
+      <c r="B42" s="14">
+        <v>14</v>
+      </c>
+      <c r="C42" s="14">
+        <v>1</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1</v>
+      </c>
+      <c r="E42" s="14">
+        <v>1946</v>
+      </c>
+      <c r="F42" s="14">
+        <v>23772745</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L42" s="14">
+        <v>33803</v>
+      </c>
+      <c r="M42" s="14">
+        <v>154578</v>
+      </c>
+      <c r="N42" s="15">
+        <v>139.35</v>
+      </c>
+      <c r="O42" s="14">
+        <v>190</v>
+      </c>
+      <c r="P42" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
+        <v>7</v>
+      </c>
+      <c r="B43" s="14">
+        <v>15</v>
+      </c>
+      <c r="C43" s="14">
+        <v>17</v>
+      </c>
+      <c r="D43" s="14">
+        <v>7</v>
+      </c>
+      <c r="E43" s="14">
+        <v>1939</v>
+      </c>
+      <c r="F43" s="14">
+        <v>23772753</v>
+      </c>
+      <c r="G43" s="14">
+        <v>448.31</v>
+      </c>
+      <c r="H43" s="15">
+        <f>G43*0.3048</f>
+        <v>136.64488800000001</v>
+      </c>
+      <c r="I43" s="15">
+        <v>459.91</v>
+      </c>
+      <c r="J43" s="15">
+        <f>I43*0.3048</f>
+        <v>140.18056800000002</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="14">
+        <v>32345</v>
+      </c>
+      <c r="M43" s="14">
+        <v>49169</v>
+      </c>
+      <c r="N43" s="15">
+        <v>140.29</v>
+      </c>
+      <c r="O43" s="14">
+        <v>190</v>
+      </c>
+      <c r="P43" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <v>1939</v>
+      </c>
+      <c r="F44">
+        <v>23772753</v>
+      </c>
+      <c r="K44" t="s">
+        <v>7</v>
+      </c>
+      <c r="L44">
+        <v>32743</v>
+      </c>
+      <c r="M44">
+        <v>116029</v>
+      </c>
+      <c r="N44" s="2">
+        <v>142.27000000000001</v>
+      </c>
+      <c r="O44">
+        <v>190</v>
+      </c>
+      <c r="P44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <v>1939</v>
+      </c>
+      <c r="F45">
+        <v>23772753</v>
+      </c>
+      <c r="K45" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45">
+        <v>32723</v>
+      </c>
+      <c r="M45">
+        <v>153748</v>
+      </c>
+      <c r="N45" s="2">
+        <v>144.02000000000001</v>
+      </c>
+      <c r="O45">
+        <v>190</v>
+      </c>
+      <c r="P45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>1928</v>
+      </c>
+      <c r="F46">
+        <v>23772755</v>
+      </c>
+      <c r="K46" t="s">
+        <v>7</v>
+      </c>
+      <c r="L46">
+        <v>32289</v>
+      </c>
+      <c r="M46">
+        <v>81849</v>
+      </c>
+      <c r="N46" s="2">
+        <v>141.33000000000001</v>
+      </c>
+      <c r="O46">
+        <v>190</v>
+      </c>
+      <c r="P46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <v>1928</v>
+      </c>
+      <c r="F47">
+        <v>23772755</v>
+      </c>
+      <c r="K47" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>32312</v>
+      </c>
+      <c r="M47">
+        <v>39872</v>
+      </c>
+      <c r="N47" s="2">
+        <v>142.86000000000001</v>
+      </c>
+      <c r="O47">
+        <v>190</v>
+      </c>
+      <c r="P47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <v>1928</v>
+      </c>
+      <c r="F48">
+        <v>23772755</v>
+      </c>
+      <c r="K48" t="s">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>32293</v>
+      </c>
+      <c r="M48">
+        <v>44564</v>
+      </c>
+      <c r="N48" s="2">
+        <v>144.02000000000001</v>
+      </c>
+      <c r="O48">
+        <v>190</v>
+      </c>
+      <c r="P48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>1928</v>
+      </c>
+      <c r="F49">
+        <v>23772755</v>
+      </c>
+      <c r="K49" t="s">
+        <v>7</v>
+      </c>
+      <c r="L49">
+        <v>32286</v>
+      </c>
+      <c r="M49">
+        <v>55945</v>
+      </c>
+      <c r="N49" s="2">
+        <v>145</v>
+      </c>
+      <c r="O49">
+        <v>190</v>
+      </c>
+      <c r="P49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>15</v>
+      </c>
+      <c r="E50">
+        <v>1928</v>
+      </c>
+      <c r="F50">
+        <v>23772755</v>
+      </c>
+      <c r="K50" t="s">
+        <v>7</v>
+      </c>
+      <c r="L50">
+        <v>32245</v>
+      </c>
+      <c r="M50">
+        <v>44971</v>
+      </c>
+      <c r="N50" s="2">
+        <v>145.02000000000001</v>
+      </c>
+      <c r="O50">
+        <v>190</v>
+      </c>
+      <c r="P50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>15</v>
+      </c>
+      <c r="E51">
+        <v>1928</v>
+      </c>
+      <c r="F51">
+        <v>23772755</v>
+      </c>
+      <c r="G51">
+        <v>456.51</v>
+      </c>
+      <c r="H51" s="2">
+        <f>G51*0.3048</f>
+        <v>139.144248</v>
+      </c>
+      <c r="I51">
+        <v>459.54</v>
+      </c>
+      <c r="J51" s="2">
+        <f>I51*0.3048</f>
+        <v>140.06779200000003</v>
+      </c>
+      <c r="K51" t="s">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>32225</v>
+      </c>
+      <c r="M51">
+        <v>40802</v>
+      </c>
+      <c r="N51" s="2">
+        <v>145.81</v>
+      </c>
+      <c r="O51">
+        <v>190</v>
+      </c>
+      <c r="P51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="E52">
+        <v>1941</v>
+      </c>
+      <c r="F52">
+        <v>23772757</v>
+      </c>
+      <c r="K52" t="s">
+        <v>7</v>
+      </c>
+      <c r="L52">
+        <v>32280</v>
+      </c>
+      <c r="M52">
+        <v>82100</v>
+      </c>
+      <c r="N52" s="2">
+        <v>141.9</v>
+      </c>
+      <c r="O52">
+        <v>190</v>
+      </c>
+      <c r="P52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>1821</v>
+      </c>
+      <c r="F53">
+        <v>23772759</v>
+      </c>
+      <c r="K53" t="s">
+        <v>7</v>
+      </c>
+      <c r="L53">
+        <v>32250</v>
+      </c>
+      <c r="M53">
+        <v>115890</v>
+      </c>
+      <c r="N53" s="2">
+        <v>141.88999999999999</v>
+      </c>
+      <c r="O53">
+        <v>190</v>
+      </c>
+      <c r="P53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>1821</v>
+      </c>
+      <c r="F54">
+        <v>23772759</v>
+      </c>
+      <c r="K54" t="s">
+        <v>7</v>
+      </c>
+      <c r="L54">
+        <v>31837</v>
+      </c>
+      <c r="M54">
+        <v>404169</v>
+      </c>
+      <c r="N54" s="2">
+        <v>142.29</v>
+      </c>
+      <c r="O54">
+        <v>190</v>
+      </c>
+      <c r="P54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>15</v>
+      </c>
+      <c r="E55">
+        <v>1821</v>
+      </c>
+      <c r="F55">
+        <v>23772759</v>
+      </c>
+      <c r="K55" t="s">
+        <v>7</v>
+      </c>
+      <c r="L55">
+        <v>32193</v>
+      </c>
+      <c r="M55">
+        <v>57042</v>
+      </c>
+      <c r="N55" s="2">
+        <v>142.56</v>
+      </c>
+      <c r="O55">
+        <v>190</v>
+      </c>
+      <c r="P55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>15</v>
+      </c>
+      <c r="E56" s="13">
+        <v>1909</v>
+      </c>
+      <c r="F56">
+        <v>23772761</v>
+      </c>
+      <c r="K56" t="s">
+        <v>7</v>
+      </c>
+      <c r="L56" s="13">
+        <v>31796</v>
+      </c>
+      <c r="M56">
+        <v>29765</v>
+      </c>
+      <c r="N56" s="2">
+        <v>143.07</v>
+      </c>
+      <c r="O56">
+        <v>190</v>
+      </c>
+      <c r="P56" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>15</v>
+      </c>
+      <c r="E57">
+        <v>1848</v>
+      </c>
+      <c r="F57">
+        <v>23772763</v>
+      </c>
+      <c r="K57" t="s">
+        <v>7</v>
+      </c>
+      <c r="L57">
+        <v>31811</v>
+      </c>
+      <c r="M57">
+        <v>142161</v>
+      </c>
+      <c r="N57" s="2">
+        <v>144.25</v>
+      </c>
+      <c r="O57">
+        <v>190</v>
+      </c>
+      <c r="P57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>1848</v>
+      </c>
+      <c r="F58">
+        <v>23772763</v>
+      </c>
+      <c r="K58" t="s">
+        <v>7</v>
+      </c>
+      <c r="L58">
+        <v>31703</v>
+      </c>
+      <c r="M58">
+        <v>46987</v>
+      </c>
+      <c r="N58" s="2">
+        <v>145.16999999999999</v>
+      </c>
+      <c r="O58">
+        <v>190</v>
+      </c>
+      <c r="P58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>15</v>
+      </c>
+      <c r="E59">
+        <v>1777</v>
+      </c>
+      <c r="F59">
+        <v>23772765</v>
+      </c>
+      <c r="K59" t="s">
+        <v>7</v>
+      </c>
+      <c r="L59">
+        <v>32208</v>
+      </c>
+      <c r="M59">
+        <v>112978</v>
+      </c>
+      <c r="N59" s="2">
+        <v>145.49</v>
+      </c>
+      <c r="O59">
+        <v>190</v>
+      </c>
+      <c r="P59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14">
+        <v>2</v>
+      </c>
+      <c r="B60" s="14">
+        <v>16</v>
+      </c>
+      <c r="C60" s="14">
+        <v>5</v>
+      </c>
+      <c r="D60" s="14">
+        <v>2</v>
+      </c>
+      <c r="E60" s="14">
+        <v>1777</v>
+      </c>
+      <c r="F60" s="14">
+        <v>23772765</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L60" s="14">
+        <v>31765</v>
+      </c>
+      <c r="M60" s="14">
+        <v>24553</v>
+      </c>
+      <c r="N60" s="15">
+        <v>148.16999999999999</v>
+      </c>
+      <c r="O60" s="14">
+        <v>190</v>
+      </c>
+      <c r="P60" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>16</v>
+      </c>
+      <c r="E61">
+        <v>1777</v>
+      </c>
+      <c r="F61">
+        <v>23772765</v>
+      </c>
+      <c r="K61" t="s">
+        <v>7</v>
+      </c>
+      <c r="L61">
+        <v>31801</v>
+      </c>
+      <c r="M61">
+        <v>33230</v>
+      </c>
+      <c r="N61" s="2">
+        <v>150.56</v>
+      </c>
+      <c r="O61">
+        <v>190</v>
+      </c>
+      <c r="P61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>16</v>
+      </c>
+      <c r="E62">
+        <v>1777</v>
+      </c>
+      <c r="F62">
+        <v>23772765</v>
+      </c>
+      <c r="K62" t="s">
+        <v>7</v>
+      </c>
+      <c r="L62">
+        <v>31763</v>
+      </c>
+      <c r="M62">
+        <v>33344</v>
+      </c>
+      <c r="N62" s="2">
+        <v>149.97</v>
+      </c>
+      <c r="O62">
+        <v>190</v>
+      </c>
+      <c r="P62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <v>1777</v>
+      </c>
+      <c r="F63">
+        <v>23772765</v>
+      </c>
+      <c r="K63" t="s">
+        <v>7</v>
+      </c>
+      <c r="L63">
+        <v>31705</v>
+      </c>
+      <c r="M63">
+        <v>22260</v>
+      </c>
+      <c r="N63" s="2">
+        <v>149.04</v>
+      </c>
+      <c r="O63">
+        <v>190</v>
+      </c>
+      <c r="P63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>1881</v>
+      </c>
+      <c r="F64">
+        <v>23774369</v>
+      </c>
+      <c r="K64" t="s">
+        <v>21</v>
+      </c>
+      <c r="L64">
+        <v>32211</v>
+      </c>
+      <c r="M64">
+        <v>87211</v>
+      </c>
+      <c r="N64" s="2">
+        <v>149.16</v>
+      </c>
+      <c r="O64">
+        <v>190</v>
+      </c>
+      <c r="P64" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="14">
+        <v>1</v>
+      </c>
+      <c r="B65" s="14">
+        <v>17</v>
+      </c>
+      <c r="C65" s="14">
+        <v>1</v>
+      </c>
+      <c r="D65" s="14">
+        <v>1</v>
+      </c>
+      <c r="E65" s="14">
+        <v>1816</v>
+      </c>
+      <c r="F65" s="14">
+        <v>23774413</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" s="14">
+        <v>31325</v>
+      </c>
+      <c r="M65" s="14">
+        <v>78961</v>
+      </c>
+      <c r="N65" s="15">
+        <v>161.96</v>
+      </c>
+      <c r="O65" s="14">
+        <v>190</v>
+      </c>
+      <c r="P65" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="14">
+        <v>1</v>
+      </c>
+      <c r="B66" s="14">
+        <v>18</v>
+      </c>
+      <c r="C66" s="14">
+        <v>1</v>
+      </c>
+      <c r="D66" s="14">
+        <v>1</v>
+      </c>
+      <c r="E66" s="14">
+        <v>2344</v>
+      </c>
+      <c r="F66" s="14">
+        <v>23773619</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L66" s="14">
+        <v>40260</v>
+      </c>
+      <c r="M66" s="14">
+        <v>412877</v>
+      </c>
+      <c r="N66" s="15">
+        <v>538.92999999999995</v>
+      </c>
+      <c r="O66" s="14">
+        <v>190</v>
+      </c>
+      <c r="P66" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <f>WETL_ID!A23</f>
+        <v>19</v>
+      </c>
+      <c r="C67">
+        <f>WETL_ID!G23</f>
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <f>WETL_ID!C23</f>
+        <v>8121</v>
+      </c>
+      <c r="F67">
+        <f>WETL_ID!E23</f>
+        <v>23809000</v>
+      </c>
+      <c r="K67" t="str">
+        <f>WETL_ID!F23</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L67">
+        <f>WETL_ID!B23</f>
+        <v>149851</v>
+      </c>
+      <c r="M67">
+        <v>50633</v>
+      </c>
+      <c r="N67" s="2">
+        <f>WETL_ID!D23</f>
+        <v>5.81</v>
+      </c>
+      <c r="O67">
+        <v>190</v>
+      </c>
+      <c r="P67" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <f>WETL_ID!A24</f>
+        <v>20</v>
+      </c>
+      <c r="C68">
+        <f>WETL_ID!G24</f>
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <f>WETL_ID!C24</f>
+        <v>8121</v>
+      </c>
+      <c r="F68">
+        <f>WETL_ID!E24</f>
+        <v>23809000</v>
+      </c>
+      <c r="K68" t="str">
+        <f>WETL_ID!F24</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L68">
+        <f>WETL_ID!B24</f>
+        <v>150311</v>
+      </c>
+      <c r="M68">
+        <v>30651</v>
+      </c>
+      <c r="N68" s="2">
+        <f>WETL_ID!D24</f>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="O68">
+        <v>190</v>
+      </c>
+      <c r="P68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <f>WETL_ID!A25</f>
+        <v>21</v>
+      </c>
+      <c r="C69">
+        <f>WETL_ID!G25</f>
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <f>WETL_ID!C25</f>
+        <v>8210</v>
+      </c>
+      <c r="F69">
+        <f>WETL_ID!E25</f>
+        <v>23809012</v>
+      </c>
+      <c r="K69" t="str">
+        <f>WETL_ID!F25</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L69">
+        <f>WETL_ID!B25</f>
+        <v>151931</v>
+      </c>
+      <c r="M69">
+        <v>114846</v>
+      </c>
+      <c r="N69" s="2">
+        <f>WETL_ID!D25</f>
+        <v>24.45</v>
+      </c>
+      <c r="O69">
+        <v>190</v>
+      </c>
+      <c r="P69" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <f>WETL_ID!A26</f>
+        <v>22</v>
+      </c>
+      <c r="C70">
+        <f>WETL_ID!G26</f>
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <f>WETL_ID!C26</f>
+        <v>8048</v>
+      </c>
+      <c r="F70">
+        <f>WETL_ID!E26</f>
+        <v>23809054</v>
+      </c>
+      <c r="K70" t="str">
+        <f>WETL_ID!F26</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L70">
+        <f>WETL_ID!B26</f>
+        <v>150784</v>
+      </c>
+      <c r="M70">
+        <v>156359</v>
+      </c>
+      <c r="N70" s="2">
+        <f>WETL_ID!D26</f>
+        <v>49.54</v>
+      </c>
+      <c r="O70">
+        <v>190</v>
+      </c>
+      <c r="P70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <f>WETL_ID!A27</f>
+        <v>23</v>
+      </c>
+      <c r="C71">
+        <f>WETL_ID!G27</f>
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <f>WETL_ID!C27</f>
+        <v>8048</v>
+      </c>
+      <c r="F71">
+        <f>WETL_ID!E27</f>
+        <v>23809054</v>
+      </c>
+      <c r="K71" t="str">
+        <f>WETL_ID!F27</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L71">
+        <f>WETL_ID!B27</f>
+        <v>150309</v>
+      </c>
+      <c r="M71">
+        <v>82608</v>
+      </c>
+      <c r="N71" s="2">
+        <f>WETL_ID!D27</f>
+        <v>51.41</v>
+      </c>
+      <c r="O71">
+        <v>190</v>
+      </c>
+      <c r="P71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <f>WETL_ID!A28</f>
+        <v>24</v>
+      </c>
+      <c r="C72">
+        <f>WETL_ID!G28</f>
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <f>WETL_ID!C28</f>
+        <v>8048</v>
+      </c>
+      <c r="F72">
+        <f>WETL_ID!E28</f>
+        <v>23809054</v>
+      </c>
+      <c r="K72" t="str">
+        <f>WETL_ID!F28</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L72">
+        <f>WETL_ID!B28</f>
+        <v>150066</v>
+      </c>
+      <c r="M72">
+        <v>114536</v>
+      </c>
+      <c r="N72" s="2">
+        <f>WETL_ID!D28</f>
+        <v>53.87</v>
+      </c>
+      <c r="O72">
+        <v>190</v>
+      </c>
+      <c r="P72" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <f>WETL_ID!A29</f>
+        <v>25</v>
+      </c>
+      <c r="C73">
+        <f>WETL_ID!G29</f>
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <f>WETL_ID!C29</f>
+        <v>8059</v>
+      </c>
+      <c r="F73">
+        <f>WETL_ID!E29</f>
+        <v>23809058</v>
+      </c>
+      <c r="K73" t="str">
+        <f>WETL_ID!F29</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L73">
+        <f>WETL_ID!B29</f>
+        <v>149542</v>
+      </c>
+      <c r="M73">
+        <v>56060</v>
+      </c>
+      <c r="N73" s="2">
+        <f>WETL_ID!D29</f>
+        <v>56.61</v>
+      </c>
+      <c r="O73">
+        <v>190</v>
+      </c>
+      <c r="P73" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <f>WETL_ID!A30</f>
+        <v>26</v>
+      </c>
+      <c r="C74">
+        <f>WETL_ID!G30</f>
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <f>WETL_ID!C30</f>
+        <v>8362</v>
+      </c>
+      <c r="F74">
+        <f>WETL_ID!E30</f>
+        <v>23815518</v>
+      </c>
+      <c r="L74">
+        <f>WETL_ID!B30</f>
+        <v>153673</v>
+      </c>
+      <c r="M74">
+        <v>52785</v>
+      </c>
+      <c r="N74" s="2">
+        <f>WETL_ID!D30</f>
+        <v>252.65</v>
+      </c>
+      <c r="O74">
+        <v>190</v>
+      </c>
+      <c r="P74" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <f>WETL_ID!A31</f>
+        <v>27</v>
+      </c>
+      <c r="C75">
+        <f>WETL_ID!G31</f>
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <f>WETL_ID!C31</f>
+        <v>8513</v>
+      </c>
+      <c r="F75">
+        <f>WETL_ID!E31</f>
+        <v>23815444</v>
+      </c>
+      <c r="K75" t="str">
+        <f>WETL_ID!F31</f>
+        <v>Crystal Springs Cr</v>
+      </c>
+      <c r="L75">
+        <f>WETL_ID!B31</f>
+        <v>156391</v>
+      </c>
+      <c r="M75">
+        <v>55853</v>
+      </c>
+      <c r="N75" s="2">
+        <f>WETL_ID!D31</f>
+        <v>30.94</v>
+      </c>
+      <c r="O75">
+        <v>190</v>
+      </c>
+      <c r="P75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <f>WETL_ID!A32</f>
+        <v>28</v>
+      </c>
+      <c r="C76">
+        <f>WETL_ID!G32</f>
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <f>WETL_ID!C32</f>
+        <v>8491</v>
+      </c>
+      <c r="F76">
+        <f>WETL_ID!E32</f>
+        <v>23815070</v>
+      </c>
+      <c r="K76" t="str">
+        <f>WETL_ID!F32</f>
+        <v>Johnson Cr</v>
+      </c>
+      <c r="L76">
+        <f>WETL_ID!B32</f>
+        <v>156910</v>
+      </c>
+      <c r="M76">
+        <v>67222</v>
+      </c>
+      <c r="N76" s="2">
+        <f>WETL_ID!D32</f>
+        <v>95.08</v>
+      </c>
+      <c r="O76">
+        <v>190</v>
+      </c>
+      <c r="P76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <f>WETL_ID!A33</f>
+        <v>29</v>
+      </c>
+      <c r="C77">
+        <f>WETL_ID!G33</f>
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <f>WETL_ID!C33</f>
+        <v>7855</v>
+      </c>
+      <c r="F77">
+        <f>WETL_ID!E33</f>
+        <v>23809078</v>
+      </c>
+      <c r="K77" t="str">
+        <f>WETL_ID!F33</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L77">
+        <f>WETL_ID!B33</f>
+        <v>145278</v>
+      </c>
+      <c r="M77">
+        <v>102588</v>
+      </c>
+      <c r="N77" s="2">
+        <f>WETL_ID!D33</f>
+        <v>86.9</v>
+      </c>
+      <c r="O77">
+        <v>190</v>
+      </c>
+      <c r="P77" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <f>WETL_ID!A34</f>
+        <v>30</v>
+      </c>
+      <c r="C78">
+        <f>WETL_ID!G34</f>
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <f>WETL_ID!C34</f>
+        <v>6766</v>
+      </c>
+      <c r="F78">
+        <f>WETL_ID!E34</f>
+        <v>23809418</v>
+      </c>
+      <c r="K78" t="str">
+        <f>WETL_ID!F34</f>
+        <v>Oak Grove Fork Clackamas R</v>
+      </c>
+      <c r="L78">
+        <f>WETL_ID!B34</f>
+        <v>120758</v>
+      </c>
+      <c r="M78">
+        <v>65830</v>
+      </c>
+      <c r="N78" s="2">
+        <f>WETL_ID!D34</f>
+        <v>665.6</v>
+      </c>
+      <c r="O78">
+        <v>190</v>
+      </c>
+      <c r="P78" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B79" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f>SUM(A1:A66)</f>
+        <v>36</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E81">
+        <v>8177</v>
+      </c>
+      <c r="F81">
+        <v>23809010</v>
+      </c>
+      <c r="K81" t="s">
+        <v>29</v>
+      </c>
+      <c r="L81">
+        <v>151913</v>
+      </c>
+      <c r="M81">
+        <v>48461</v>
+      </c>
+      <c r="N81" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="O81">
+        <v>190</v>
+      </c>
+      <c r="P81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E82">
+        <v>8121</v>
+      </c>
+      <c r="F82">
+        <f>WETL_ID!E25</f>
+        <v>23809012</v>
+      </c>
+      <c r="K82" t="str">
+        <f>WETL_ID!F25</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L82">
+        <v>150532</v>
+      </c>
+      <c r="M82">
+        <v>115205</v>
+      </c>
+      <c r="N82" s="2">
+        <v>12.75</v>
+      </c>
+      <c r="O82">
+        <v>190</v>
+      </c>
+      <c r="P82" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E83">
+        <v>8121</v>
+      </c>
+      <c r="F83">
+        <f>WETL_ID!E26</f>
+        <v>23809054</v>
+      </c>
+      <c r="K83" t="str">
+        <f>WETL_ID!F26</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L83">
+        <v>150537</v>
+      </c>
+      <c r="M83">
+        <v>73350</v>
+      </c>
+      <c r="N83" s="2">
+        <v>11.84</v>
+      </c>
+      <c r="O83">
+        <v>190</v>
+      </c>
+      <c r="P83" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E84">
+        <v>8210</v>
+      </c>
+      <c r="F84">
+        <f>WETL_ID!E27</f>
+        <v>23809054</v>
+      </c>
+      <c r="K84" t="str">
+        <f>WETL_ID!F27</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L84">
+        <v>151868</v>
+      </c>
+      <c r="M84">
+        <v>36088</v>
+      </c>
+      <c r="N84" s="2">
+        <v>26.37</v>
+      </c>
+      <c r="O84">
+        <v>190</v>
+      </c>
+      <c r="P84" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E85">
+        <v>8210</v>
+      </c>
+      <c r="F85">
+        <f>WETL_ID!E28</f>
+        <v>23809054</v>
+      </c>
+      <c r="K85" t="str">
+        <f>WETL_ID!F28</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L85">
+        <v>151932</v>
+      </c>
+      <c r="M85">
+        <v>158531</v>
+      </c>
+      <c r="N85" s="2">
+        <v>34.33</v>
+      </c>
+      <c r="O85">
+        <v>190</v>
+      </c>
+      <c r="P85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E86">
+        <v>8048</v>
+      </c>
+      <c r="F86">
+        <f>WETL_ID!E27</f>
+        <v>23809054</v>
+      </c>
+      <c r="K86" t="str">
+        <f>WETL_ID!F27</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L86">
+        <v>150597</v>
+      </c>
+      <c r="M86">
+        <v>129261</v>
+      </c>
+      <c r="N86" s="2">
+        <v>49.96</v>
+      </c>
+      <c r="O86">
+        <v>190</v>
+      </c>
+      <c r="P86" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E87">
+        <v>8048</v>
+      </c>
+      <c r="F87">
+        <v>23809054</v>
+      </c>
+      <c r="K87" t="s">
+        <v>29</v>
+      </c>
+      <c r="L87">
+        <v>150308</v>
+      </c>
+      <c r="M87">
+        <v>63243</v>
+      </c>
+      <c r="N87" s="2">
+        <v>53.65</v>
+      </c>
+      <c r="O87">
+        <v>190</v>
+      </c>
+      <c r="P87" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E88">
+        <v>8048</v>
+      </c>
+      <c r="F88">
+        <f>WETL_ID!E28</f>
+        <v>23809054</v>
+      </c>
+      <c r="K88" t="str">
+        <f>WETL_ID!F28</f>
+        <v>Clackamas R</v>
+      </c>
+      <c r="L88">
+        <v>150374</v>
+      </c>
+      <c r="M88">
+        <v>111581</v>
+      </c>
+      <c r="N88" s="2">
+        <v>54.99</v>
+      </c>
+      <c r="O88">
+        <v>190</v>
+      </c>
+      <c r="P88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E89">
+        <v>8032</v>
+      </c>
+      <c r="F89">
+        <v>23809056</v>
+      </c>
+      <c r="K89" t="s">
+        <v>29</v>
+      </c>
+      <c r="L89">
+        <v>149886</v>
+      </c>
+      <c r="M89">
+        <v>31686</v>
+      </c>
+      <c r="N89" s="2">
+        <v>55.48</v>
+      </c>
+      <c r="O89">
+        <v>190</v>
+      </c>
+      <c r="P89" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="90" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E90">
+        <v>8032</v>
+      </c>
+      <c r="F90">
+        <v>23809056</v>
+      </c>
+      <c r="K90" t="s">
+        <v>29</v>
+      </c>
+      <c r="L90">
+        <v>149599</v>
+      </c>
+      <c r="M90">
+        <v>30277</v>
+      </c>
+      <c r="N90" s="2">
+        <v>56.36</v>
+      </c>
+      <c r="O90">
+        <v>190</v>
+      </c>
+      <c r="P90" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="91" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E91">
+        <v>8059</v>
+      </c>
+      <c r="F91">
+        <v>23809058</v>
+      </c>
+      <c r="K91" t="s">
+        <v>29</v>
+      </c>
+      <c r="L91">
+        <v>149302</v>
+      </c>
+      <c r="M91">
+        <v>106965</v>
+      </c>
+      <c r="N91" s="2">
+        <v>58.03</v>
+      </c>
+      <c r="O91">
+        <v>190</v>
+      </c>
+      <c r="P91" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E92">
+        <v>8059</v>
+      </c>
+      <c r="F92">
+        <v>23809058</v>
+      </c>
+      <c r="K92" t="s">
+        <v>29</v>
+      </c>
+      <c r="L92">
+        <v>149553</v>
+      </c>
+      <c r="M92">
+        <v>108892</v>
+      </c>
+      <c r="N92" s="2">
+        <v>57.66</v>
+      </c>
+      <c r="O92">
+        <v>190</v>
+      </c>
+      <c r="P92" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E93">
+        <v>8059</v>
+      </c>
+      <c r="F93">
+        <v>23809058</v>
+      </c>
+      <c r="K93" t="s">
+        <v>29</v>
+      </c>
+      <c r="L93">
+        <v>149525</v>
+      </c>
+      <c r="M93">
+        <v>26723</v>
+      </c>
+      <c r="N93" s="2">
+        <v>60.11</v>
+      </c>
+      <c r="O93">
+        <v>190</v>
+      </c>
+      <c r="P93" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <v>8059</v>
+      </c>
+      <c r="F94">
+        <v>23809058</v>
+      </c>
+      <c r="K94" t="s">
+        <v>29</v>
+      </c>
+      <c r="L94">
+        <v>149394</v>
+      </c>
+      <c r="M94">
+        <v>46447</v>
+      </c>
+      <c r="N94" s="2">
+        <v>56.94</v>
+      </c>
+      <c r="O94">
+        <v>190</v>
+      </c>
+      <c r="P94" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="L95" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M95" s="4">
+        <f>SUM(M90:M94)/10000</f>
+        <v>31.930399999999999</v>
+      </c>
+      <c r="N95" s="2">
+        <f>SUMPRODUCT(M90:M94,N90:N94)/(M95*10000)</f>
+        <v>57.760989840402878</v>
+      </c>
+      <c r="O95" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="5:17" x14ac:dyDescent="0.3">
+      <c r="N96"/>
+    </row>
+    <row r="97" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L97" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M97" s="4">
+        <f>SUM(M95:M96)/10000</f>
+        <v>3.1930399999999999E-3</v>
+      </c>
+      <c r="N97" s="2">
+        <f>SUMPRODUCT(M95:M96,N95:N96)/(M97*10000)</f>
+        <v>57.760989840402878</v>
+      </c>
+      <c r="O97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L99" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M99" s="4">
+        <f>SUM(M95:M98)/10000</f>
+        <v>3.1933593039999999E-3</v>
+      </c>
+      <c r="N99" s="2">
+        <f>SUMPRODUCT(M95:M98,N95:N98)/(M99*10000)</f>
+        <v>57.760989840402878</v>
+      </c>
+      <c r="O99" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L101" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M101" s="4">
+        <f>SUM(M99:M100)/10000</f>
+        <v>3.1933593039999999E-7</v>
+      </c>
+      <c r="N101" s="2">
+        <f>SUMPRODUCT(M99:M100,N99:N100)/(M101*10000)</f>
+        <v>57.760989840402878</v>
+      </c>
+      <c r="O101" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L103" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M103" s="4">
+        <f>SUM(M100:M102)/10000</f>
+        <v>3.1933593039999998E-11</v>
+      </c>
+      <c r="N103" s="2">
+        <f>SUMPRODUCT(M100:M102,N100:N102)/(M103*10000)</f>
+        <v>57.760989840402878</v>
+      </c>
+      <c r="O103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L105" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M105" s="4">
+        <f>SUM(M104:M104)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N105" s="2" t="e">
+        <f>SUMPRODUCT(M104:M104,N104:N104)/(M105*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O105" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L107" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M107" s="4">
+        <f>SUM(M102:M106)/10000</f>
+        <v>3.1933593039999997E-15</v>
+      </c>
+      <c r="N107" s="2" t="e">
+        <f>SUMPRODUCT(M102:M106,N102:N106)/(M107*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O107" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L109" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M109" s="4">
+        <f>SUM(M108:M108)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N109" s="2" t="e">
+        <f>SUMPRODUCT(M108:M108,N108:N108)/(M109*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O109" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L111" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M111" s="4">
+        <f>SUM(M108:M110)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N111" s="2" t="e">
+        <f>SUMPRODUCT(M108:M110,N108:N110)/(M111*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O111" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L113" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M113" s="4">
+        <f>SUM(M111:M112)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N113" s="2" t="e">
+        <f>SUMPRODUCT(M111:M112,N111:N112)/(M113*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O113" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L115" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M115" s="4">
+        <f>SUM(M109:M114)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N115" s="2" t="e">
+        <f>SUMPRODUCT(M109:M114,N109:N114)/(M115*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O115" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L117" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M117" s="4">
+        <f>SUM(M112:M116)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N117" s="3" t="e">
+        <f>SUMPRODUCT(M112:M116,N112:N116)/((M117-M115/10000)*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O117" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L119" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M119" s="4">
+        <f>SUM(M118:M118)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N119" s="2" t="e">
+        <f>SUMPRODUCT(M118:M118,N118:N118)/(M119*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O119" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="121" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L121" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M121" s="4">
+        <f>SUM(M120:M120)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N121" s="2" t="e">
+        <f>SUMPRODUCT(M120:M120,N120:N120)/(M121*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O121" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L123" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M123" s="4">
+        <f>SUM(M106:M122)/10000</f>
+        <v>3.1933593039999998E-19</v>
+      </c>
+      <c r="N123" s="2" t="e">
+        <f>SUMPRODUCT(M106:M122,N106:N122)/(M123*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O123" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L125" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M125" s="4">
+        <f>SUM(M120:M124)/10000</f>
+        <v>3.1933593039999998E-23</v>
+      </c>
+      <c r="N125" s="2" t="e">
+        <f>SUMPRODUCT(M120:M124,N120:N124)/(M125*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O125" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L127" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M127" s="4">
+        <f>SUM(M126:M126)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N127" s="2" t="e">
+        <f>SUMPRODUCT(M126:M126,N126:N126)/(M127*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O127" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="128" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L128" s="5"/>
+      <c r="M128" s="4"/>
+    </row>
+    <row r="129" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L129" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M129" s="4">
+        <f>SUM(M128:M128)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N129" s="2" t="e">
+        <f>SUMPRODUCT(M128:M128,N128:N128)/(M129*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O129" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="130" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <f>SUM(C29:C129)</f>
+        <v>63</v>
+      </c>
+      <c r="L130" s="5"/>
+      <c r="M130" s="4"/>
+    </row>
+    <row r="132" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L132" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M132" s="4">
+        <f>SUM(M129:M131)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N132" s="2" t="e">
+        <f>SUMPRODUCT(M129:M131,N129:N131)/(M132*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O132" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="133" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L133" s="5"/>
+      <c r="M133" s="4"/>
+    </row>
+    <row r="134" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L134" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M134" s="4">
+        <f>SUM(M130:M133)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N134" s="2" t="e">
+        <f>SUMPRODUCT(M130:M133,N130:N133)/(M134*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O134" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L135" s="5"/>
+      <c r="M135" s="4"/>
+    </row>
+    <row r="136" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L136" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M136" s="4">
+        <f>SUM(M134:M135)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N136" s="2" t="e">
+        <f>SUMPRODUCT(M134:M135,N134:N135)/(M136*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O136" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="137" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L137" s="5"/>
+      <c r="M137" s="4"/>
+    </row>
+    <row r="138" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L138" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M138" s="4">
+        <f>SUM(M135:M137)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N138" s="2" t="e">
+        <f>SUMPRODUCT(M135:M137,N135:N137)/(M138*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O138" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L139" s="5"/>
+      <c r="M139" s="4"/>
+    </row>
+    <row r="140" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L140" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M140" s="4">
+        <f>SUM(M138:M139)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N140" s="2" t="e">
+        <f>SUMPRODUCT(M138:M139,N138:N139)/(M140*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O140" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L141" s="5"/>
+      <c r="M141" s="4"/>
+    </row>
+    <row r="142" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L142" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M142" s="4">
+        <f>SUM(M136:M141)/10000</f>
+        <v>0</v>
+      </c>
+      <c r="N142" s="2" t="e">
+        <f>SUMPRODUCT(M136:M141,N136:N141)/(M142*10000)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O142" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="143" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="L143" s="5"/>
+      <c r="M143" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:Q143">
+    <sortCondition ref="B2:B143"/>
+    <sortCondition ref="F2:F143"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Limit the amount of Q2WETL that goes into each wetland IDU to the capacity of the wetland. Fix some bugs which affect HruIRRIG_SOIL and HruNAT_SOIL. CW3MdataDictionary.xlsx - Annotate HruIRRIG_SOIL and HruNAT_SOIL. FLOWreports_McKenzie.xml - Add "FLOW Wetland 10 Analysis" report. Flow.cpp, .h - Add logic to ensure that HruIRRIG_SOIL and HruNAT_SOIL are depths relative to the irrigated and non-irrigated areas of the HRU, rather than relative to the total area of the HRU. Also, limit the amount of Q2WETL that goes into each wetland IDU to the capacity of the wetland. HBV.cpp - Replace an ASSERT with a warning message.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC98C0A1-A85C-4F85-B3DE-70691774F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BF9EBF-C696-4860-BF66-3245008386B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
   <sheets>
     <sheet name="WETL_ID" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
       <pane xSplit="10" ySplit="13" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71514D07-858F-4F8F-B9B0-14D5E7A5141D}">
   <dimension ref="A1:P143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
@@ -5437,7 +5437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9225645-945C-4C81-90D4-9241866A6700}">
   <dimension ref="A1:Q143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. CW3MdataDictionary.xlsx - Add IDU attribute FLOODDEPTH.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BF9EBF-C696-4860-BF66-3245008386B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F634EF5-B3E1-41EA-9603-527A5BAE9C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
   <sheets>
     <sheet name="WETL_ID" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4153BDD9-3748-4423-B686-257FDC6E887B}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="10" ySplit="13" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71514D07-858F-4F8F-B9B0-14D5E7A5141D}">
   <dimension ref="A1:P143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
@@ -5438,8 +5438,8 @@
   <dimension ref="A1:Q143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6861,22 +6861,22 @@
         <v>15</v>
       </c>
       <c r="E44">
-        <v>1939</v>
+        <v>1848</v>
       </c>
       <c r="F44">
-        <v>23772753</v>
+        <v>23772763</v>
       </c>
       <c r="K44" t="s">
         <v>7</v>
       </c>
       <c r="L44">
-        <v>32743</v>
+        <v>31703</v>
       </c>
       <c r="M44">
-        <v>116029</v>
+        <v>46987</v>
       </c>
       <c r="N44" s="2">
-        <v>142.27000000000001</v>
+        <v>145.16999999999999</v>
       </c>
       <c r="O44">
         <v>190</v>
@@ -6889,29 +6889,32 @@
       <c r="B45">
         <v>15</v>
       </c>
-      <c r="E45">
-        <v>1939</v>
+      <c r="E45" s="13">
+        <v>1909</v>
       </c>
       <c r="F45">
-        <v>23772753</v>
+        <v>23772761</v>
       </c>
       <c r="K45" t="s">
         <v>7</v>
       </c>
-      <c r="L45">
-        <v>32723</v>
+      <c r="L45" s="13">
+        <v>31796</v>
       </c>
       <c r="M45">
-        <v>153748</v>
+        <v>29765</v>
       </c>
       <c r="N45" s="2">
-        <v>144.02000000000001</v>
+        <v>143.07</v>
       </c>
       <c r="O45">
         <v>190</v>
       </c>
       <c r="P45" t="s">
         <v>27</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
@@ -6919,22 +6922,22 @@
         <v>15</v>
       </c>
       <c r="E46">
-        <v>1928</v>
+        <v>1848</v>
       </c>
       <c r="F46">
-        <v>23772755</v>
+        <v>23772763</v>
       </c>
       <c r="K46" t="s">
         <v>7</v>
       </c>
       <c r="L46">
-        <v>32289</v>
+        <v>31811</v>
       </c>
       <c r="M46">
-        <v>81849</v>
+        <v>142161</v>
       </c>
       <c r="N46" s="2">
-        <v>141.33000000000001</v>
+        <v>144.25</v>
       </c>
       <c r="O46">
         <v>190</v>
@@ -6948,22 +6951,22 @@
         <v>15</v>
       </c>
       <c r="E47">
-        <v>1928</v>
+        <v>1821</v>
       </c>
       <c r="F47">
-        <v>23772755</v>
+        <v>23772759</v>
       </c>
       <c r="K47" t="s">
         <v>7</v>
       </c>
       <c r="L47">
-        <v>32312</v>
+        <v>31837</v>
       </c>
       <c r="M47">
-        <v>39872</v>
+        <v>404169</v>
       </c>
       <c r="N47" s="2">
-        <v>142.86000000000001</v>
+        <v>142.29</v>
       </c>
       <c r="O47">
         <v>190</v>
@@ -6977,22 +6980,22 @@
         <v>15</v>
       </c>
       <c r="E48">
-        <v>1928</v>
+        <v>1821</v>
       </c>
       <c r="F48">
-        <v>23772755</v>
+        <v>23772759</v>
       </c>
       <c r="K48" t="s">
         <v>7</v>
       </c>
       <c r="L48">
-        <v>32293</v>
+        <v>32193</v>
       </c>
       <c r="M48">
-        <v>44564</v>
+        <v>57042</v>
       </c>
       <c r="N48" s="2">
-        <v>144.02000000000001</v>
+        <v>142.56</v>
       </c>
       <c r="O48">
         <v>190</v>
@@ -7001,27 +7004,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>15</v>
       </c>
       <c r="E49">
-        <v>1928</v>
+        <v>1777</v>
       </c>
       <c r="F49">
-        <v>23772755</v>
+        <v>23772765</v>
       </c>
       <c r="K49" t="s">
         <v>7</v>
       </c>
       <c r="L49">
-        <v>32286</v>
+        <v>32208</v>
       </c>
       <c r="M49">
-        <v>55945</v>
+        <v>112978</v>
       </c>
       <c r="N49" s="2">
-        <v>145</v>
+        <v>145.49</v>
       </c>
       <c r="O49">
         <v>190</v>
@@ -7030,7 +7033,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B50">
         <v>15</v>
       </c>
@@ -7040,17 +7043,31 @@
       <c r="F50">
         <v>23772755</v>
       </c>
+      <c r="G50">
+        <v>456.51</v>
+      </c>
+      <c r="H50" s="2">
+        <f>G50*0.3048</f>
+        <v>139.144248</v>
+      </c>
+      <c r="I50">
+        <v>459.54</v>
+      </c>
+      <c r="J50" s="2">
+        <f>I50*0.3048</f>
+        <v>140.06779200000003</v>
+      </c>
       <c r="K50" t="s">
         <v>7</v>
       </c>
       <c r="L50">
-        <v>32245</v>
+        <v>32225</v>
       </c>
       <c r="M50">
-        <v>44971</v>
+        <v>40802</v>
       </c>
       <c r="N50" s="2">
-        <v>145.02000000000001</v>
+        <v>145.81</v>
       </c>
       <c r="O50">
         <v>190</v>
@@ -7059,7 +7076,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B51">
         <v>15</v>
       </c>
@@ -7069,31 +7086,17 @@
       <c r="F51">
         <v>23772755</v>
       </c>
-      <c r="G51">
-        <v>456.51</v>
-      </c>
-      <c r="H51" s="2">
-        <f>G51*0.3048</f>
-        <v>139.144248</v>
-      </c>
-      <c r="I51">
-        <v>459.54</v>
-      </c>
-      <c r="J51" s="2">
-        <f>I51*0.3048</f>
-        <v>140.06779200000003</v>
-      </c>
       <c r="K51" t="s">
         <v>7</v>
       </c>
       <c r="L51">
-        <v>32225</v>
+        <v>32245</v>
       </c>
       <c r="M51">
-        <v>40802</v>
+        <v>44971</v>
       </c>
       <c r="N51" s="2">
-        <v>145.81</v>
+        <v>145.02000000000001</v>
       </c>
       <c r="O51">
         <v>190</v>
@@ -7102,27 +7105,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B52">
         <v>15</v>
       </c>
       <c r="E52">
-        <v>1941</v>
+        <v>1821</v>
       </c>
       <c r="F52">
-        <v>23772757</v>
+        <v>23772759</v>
       </c>
       <c r="K52" t="s">
         <v>7</v>
       </c>
       <c r="L52">
-        <v>32280</v>
+        <v>32250</v>
       </c>
       <c r="M52">
-        <v>82100</v>
+        <v>115890</v>
       </c>
       <c r="N52" s="2">
-        <v>141.9</v>
+        <v>141.88999999999999</v>
       </c>
       <c r="O52">
         <v>190</v>
@@ -7131,27 +7134,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>15</v>
       </c>
       <c r="E53">
-        <v>1821</v>
+        <v>1941</v>
       </c>
       <c r="F53">
-        <v>23772759</v>
+        <v>23772757</v>
       </c>
       <c r="K53" t="s">
         <v>7</v>
       </c>
       <c r="L53">
-        <v>32250</v>
+        <v>32280</v>
       </c>
       <c r="M53">
-        <v>115890</v>
+        <v>82100</v>
       </c>
       <c r="N53" s="2">
-        <v>141.88999999999999</v>
+        <v>141.9</v>
       </c>
       <c r="O53">
         <v>190</v>
@@ -7160,27 +7163,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>15</v>
       </c>
       <c r="E54">
-        <v>1821</v>
+        <v>1928</v>
       </c>
       <c r="F54">
-        <v>23772759</v>
+        <v>23772755</v>
       </c>
       <c r="K54" t="s">
         <v>7</v>
       </c>
       <c r="L54">
-        <v>31837</v>
+        <v>32286</v>
       </c>
       <c r="M54">
-        <v>404169</v>
+        <v>55945</v>
       </c>
       <c r="N54" s="2">
-        <v>142.29</v>
+        <v>145</v>
       </c>
       <c r="O54">
         <v>190</v>
@@ -7189,27 +7192,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>15</v>
       </c>
       <c r="E55">
-        <v>1821</v>
+        <v>1928</v>
       </c>
       <c r="F55">
-        <v>23772759</v>
+        <v>23772755</v>
       </c>
       <c r="K55" t="s">
         <v>7</v>
       </c>
       <c r="L55">
-        <v>32193</v>
+        <v>32289</v>
       </c>
       <c r="M55">
-        <v>57042</v>
+        <v>81849</v>
       </c>
       <c r="N55" s="2">
-        <v>142.56</v>
+        <v>141.33000000000001</v>
       </c>
       <c r="O55">
         <v>190</v>
@@ -7218,27 +7221,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B56">
         <v>15</v>
       </c>
-      <c r="E56" s="13">
-        <v>1909</v>
+      <c r="E56">
+        <v>1928</v>
       </c>
       <c r="F56">
-        <v>23772761</v>
+        <v>23772755</v>
       </c>
       <c r="K56" t="s">
         <v>7</v>
       </c>
-      <c r="L56" s="13">
-        <v>31796</v>
+      <c r="L56">
+        <v>32293</v>
       </c>
       <c r="M56">
-        <v>29765</v>
+        <v>44564</v>
       </c>
       <c r="N56" s="2">
-        <v>143.07</v>
+        <v>144.02000000000001</v>
       </c>
       <c r="O56">
         <v>190</v>
@@ -7246,31 +7249,28 @@
       <c r="P56" t="s">
         <v>27</v>
       </c>
-      <c r="Q56" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B57">
         <v>15</v>
       </c>
       <c r="E57">
-        <v>1848</v>
+        <v>1928</v>
       </c>
       <c r="F57">
-        <v>23772763</v>
+        <v>23772755</v>
       </c>
       <c r="K57" t="s">
         <v>7</v>
       </c>
       <c r="L57">
-        <v>31811</v>
+        <v>32312</v>
       </c>
       <c r="M57">
-        <v>142161</v>
+        <v>39872</v>
       </c>
       <c r="N57" s="2">
-        <v>144.25</v>
+        <v>142.86000000000001</v>
       </c>
       <c r="O57">
         <v>190</v>
@@ -7279,27 +7279,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>15</v>
       </c>
       <c r="E58">
-        <v>1848</v>
+        <v>1939</v>
       </c>
       <c r="F58">
-        <v>23772763</v>
+        <v>23772753</v>
       </c>
       <c r="K58" t="s">
         <v>7</v>
       </c>
       <c r="L58">
-        <v>31703</v>
+        <v>32723</v>
       </c>
       <c r="M58">
-        <v>46987</v>
+        <v>153748</v>
       </c>
       <c r="N58" s="2">
-        <v>145.16999999999999</v>
+        <v>144.02000000000001</v>
       </c>
       <c r="O58">
         <v>190</v>
@@ -7308,27 +7308,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B59">
         <v>15</v>
       </c>
       <c r="E59">
-        <v>1777</v>
+        <v>1939</v>
       </c>
       <c r="F59">
-        <v>23772765</v>
+        <v>23772753</v>
       </c>
       <c r="K59" t="s">
         <v>7</v>
       </c>
       <c r="L59">
-        <v>32208</v>
+        <v>32743</v>
       </c>
       <c r="M59">
-        <v>112978</v>
+        <v>116029</v>
       </c>
       <c r="N59" s="2">
-        <v>145.49</v>
+        <v>142.27000000000001</v>
       </c>
       <c r="O59">
         <v>190</v>
@@ -7337,7 +7337,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="14">
         <v>2</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B61">
         <v>16</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>16</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B63">
         <v>16</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B64">
         <v>16</v>
       </c>
@@ -8917,9 +8917,8 @@
       <c r="M143" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:Q143">
-    <sortCondition ref="B2:B143"/>
-    <sortCondition ref="F2:F143"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A44:Q59">
+    <sortCondition ref="L44:L59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
This log also covers the previous commit. Separate FLOODDEPTH from WETNESS. CW3MdataDictionary.xlsx - Add IDU attribute FLOODDEPTH. FLOWreports_McKenzie.xml - Recode the Net kcal calculation in the "FLOW Shade-a-lator reach comparison" report. APs.cpp - Add FLOODDEPTH to RunPrescribedLULCs(). Flow.cpp - Include FLOODDEPTH in FixHRUwaterBalance(), ReachH2OtoWetlandIDU(), FlowModel::Run(), FlowModel::StartYear(), CheckHRUwaterBalance(), CheckSurfaceH2O(), and WetlSurfH2Ofluxes(). In ApplyQ2WETL(), instead of returning floodwaters to the reaches, overfill the wetland. The floodwater goes back to the reaches the next day. In ReachH2OtoWetland(), assert that FLOODDEPTH is 0 on entry. HBV.cpp - Include FLOODDEPTH when calculating surface water.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F634EF5-B3E1-41EA-9603-527A5BAE9C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C90011D-4C25-48F3-9ED3-34CA1D7CF52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15540" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
   <sheets>
     <sheet name="WETL_ID" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="IDUs (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -617,16 +618,16 @@
       <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.44140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -638,7 +639,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,7 +674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -704,7 +705,7 @@
         <v>114.80779151818864</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -735,7 +736,7 @@
         <v>115.87905496354458</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -765,7 +766,7 @@
         <v>117.99</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -796,7 +797,7 @@
         <v>120.46777268610882</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -827,7 +828,7 @@
         <v>124.10821118901781</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -858,7 +859,7 @@
         <v>122.91</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -889,7 +890,7 @@
         <v>125.35983235482429</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -917,7 +918,7 @@
         <v>128.61000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -948,7 +949,7 @@
         <v>128.65973004744384</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -979,7 +980,7 @@
         <v>131.56476101660903</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>130.65</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>134.27690288100209</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>134.74</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1102,7 +1103,7 @@
         <v>139.35</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>143.65</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>161.96</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>519.25480000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>5024523</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1318,7 +1319,7 @@
         <v>5025225</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>5027758</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>5025729</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>5025134</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1466,7 +1467,7 @@
         <v>5024842</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>5023984</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>5031580</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>5036203</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>5037421</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>5017267</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>4991642</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>203.66809999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
@@ -1736,17 +1737,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>203.6249</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>15</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>37.5364</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>18</v>
       </c>
@@ -1804,7 +1805,7 @@
         <v>35.7926</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>28.562000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>21.9206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>14.622199999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>12</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>10.258800000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>6.7222</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>6.5830000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -1916,7 +1917,7 @@
         <v>5.5853000000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>14</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>5.2785000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>5.0632999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6</v>
       </c>
@@ -1953,7 +1954,7 @@
       </c>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1961,7 +1962,7 @@
         <v>12.8376</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>10.452</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>10</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>8.4712999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>17</v>
       </c>
@@ -1985,7 +1986,7 @@
         <v>7.8960999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>13</v>
       </c>
@@ -2011,16 +2012,16 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2067,12 +2068,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2194,7 +2195,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K8" s="5" t="s">
         <v>20</v>
       </c>
@@ -2239,10 +2240,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K12" s="5" t="s">
         <v>20</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K18" s="5" t="s">
         <v>20</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2489,7 +2490,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K22" s="5" t="s">
         <v>20</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2633,7 +2634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K27" s="5" t="s">
         <v>20</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K30" s="5" t="s">
         <v>17</v>
       </c>
@@ -2700,7 +2701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2735,7 +2736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -2790,7 +2791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K37" s="5" t="s">
         <v>20</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K40" s="5" t="s">
         <v>17</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2973,7 +2974,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K45" s="5" t="s">
         <v>20</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>10</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>10</v>
       </c>
@@ -3082,7 +3083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K49" s="5" t="s">
         <v>20</v>
       </c>
@@ -3098,7 +3099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>11</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>11</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -3191,7 +3192,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -3220,7 +3221,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>11</v>
       </c>
@@ -3249,7 +3250,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>11</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K57" s="5" t="s">
         <v>20</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>12</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>12</v>
       </c>
@@ -3355,7 +3356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>12</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>12</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>12</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K64" s="5" t="s">
         <v>20</v>
       </c>
@@ -3458,7 +3459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>13</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K67" s="5" t="s">
         <v>20</v>
       </c>
@@ -3509,7 +3510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>14</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K70" s="5" t="s">
         <v>20</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>15</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>15</v>
       </c>
@@ -3638,7 +3639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15</v>
       </c>
@@ -3667,7 +3668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>15</v>
       </c>
@@ -3696,7 +3697,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15</v>
       </c>
@@ -3725,7 +3726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>15</v>
       </c>
@@ -3754,7 +3755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>15</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>15</v>
       </c>
@@ -3812,7 +3813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>15</v>
       </c>
@@ -3844,7 +3845,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>15</v>
       </c>
@@ -3873,7 +3874,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>15</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>15</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>15</v>
       </c>
@@ -3960,7 +3961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>15</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>15</v>
       </c>
@@ -4018,7 +4019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>15</v>
       </c>
@@ -4047,7 +4048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>15</v>
       </c>
@@ -4090,7 +4091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K89" s="5" t="s">
         <v>20</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>16</v>
       </c>
@@ -4144,7 +4145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>16</v>
       </c>
@@ -4173,7 +4174,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>16</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>16</v>
       </c>
@@ -4231,7 +4232,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>16</v>
       </c>
@@ -4260,7 +4261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K96" s="5" t="s">
         <v>20</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>17</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K99" s="5" t="s">
         <v>20</v>
       </c>
@@ -4327,11 +4328,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K100" s="5"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>18</v>
       </c>
@@ -4366,7 +4367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K102" s="5" t="s">
         <v>20</v>
       </c>
@@ -4382,7 +4383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B103">
         <f>SUM(B2:B102)</f>
         <v>65</v>
@@ -4390,12 +4391,12 @@
       <c r="K103" s="5"/>
       <c r="L103" s="4"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <f>WETL_ID!A23</f>
         <v>19</v>
@@ -4440,7 +4441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107">
         <f>WETL_ID!A24</f>
         <v>20</v>
@@ -4482,7 +4483,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D108">
         <v>8121</v>
       </c>
@@ -4510,7 +4511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D109">
         <v>8121</v>
       </c>
@@ -4538,7 +4539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K110" s="5" t="s">
         <v>20</v>
       </c>
@@ -4554,11 +4555,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K111" s="5"/>
       <c r="L111" s="4"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112">
         <f>WETL_ID!A25</f>
         <v>21</v>
@@ -4600,7 +4601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D113">
         <v>8177</v>
       </c>
@@ -4626,7 +4627,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D114">
         <v>8210</v>
       </c>
@@ -4654,7 +4655,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D115">
         <v>8210</v>
       </c>
@@ -4682,7 +4683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K116" s="5" t="s">
         <v>20</v>
       </c>
@@ -4698,11 +4699,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K117" s="5"/>
       <c r="L117" s="4"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118">
         <f>WETL_ID!A26</f>
         <v>22</v>
@@ -4744,7 +4745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D119">
         <v>8048</v>
       </c>
@@ -4772,7 +4773,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K120" s="5" t="s">
         <v>20</v>
       </c>
@@ -4788,11 +4789,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K121" s="5"/>
       <c r="L121" s="4"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122">
         <f>WETL_ID!A27</f>
         <v>23</v>
@@ -4834,7 +4835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D123">
         <v>8048</v>
       </c>
@@ -4860,7 +4861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D124">
         <v>8048</v>
       </c>
@@ -4888,7 +4889,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K125" s="5" t="s">
         <v>20</v>
       </c>
@@ -4904,11 +4905,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K126" s="5"/>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127">
         <f>WETL_ID!A28</f>
         <v>24</v>
@@ -4953,7 +4954,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D128">
         <v>8032</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K129" s="5" t="s">
         <v>20</v>
       </c>
@@ -4998,11 +4999,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K130" s="5"/>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131">
         <f>WETL_ID!A29</f>
         <v>25</v>
@@ -5047,7 +5048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D132">
         <v>8059</v>
       </c>
@@ -5076,7 +5077,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D133">
         <v>8059</v>
       </c>
@@ -5105,7 +5106,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D134">
         <v>8032</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D135">
         <v>8059</v>
       </c>
@@ -5163,7 +5164,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D136">
         <v>8059</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K137" s="5" t="s">
         <v>20</v>
       </c>
@@ -5208,11 +5209,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K138" s="5"/>
       <c r="L138" s="4"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139">
         <f>WETL_ID!A30</f>
         <v>26</v>
@@ -5250,7 +5251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140">
         <f>WETL_ID!A31</f>
         <v>27</v>
@@ -5292,7 +5293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141">
         <f>WETL_ID!A32</f>
         <v>28</v>
@@ -5334,7 +5335,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142">
         <f>WETL_ID!A33</f>
         <v>29</v>
@@ -5379,7 +5380,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143">
         <f>WETL_ID!A34</f>
         <v>30</v>
@@ -5442,16 +5443,16 @@
       <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>2</v>
       </c>
@@ -5539,7 +5540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5568,7 +5569,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -5597,7 +5598,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -5626,7 +5627,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -5655,7 +5656,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -5693,7 +5694,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>2</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>4</v>
       </c>
@@ -5754,7 +5755,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>3</v>
       </c>
@@ -5789,7 +5790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3</v>
       </c>
@@ -5815,7 +5816,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3</v>
       </c>
@@ -5841,7 +5842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>2</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>4</v>
       </c>
@@ -5908,7 +5909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>1</v>
       </c>
@@ -5949,7 +5950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>5</v>
       </c>
@@ -5981,7 +5982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>5</v>
       </c>
@@ -6010,7 +6011,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>1</v>
       </c>
@@ -6048,7 +6049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>4</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>7</v>
       </c>
@@ -6115,7 +6116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>7</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>7</v>
       </c>
@@ -6170,7 +6171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>7</v>
       </c>
@@ -6196,7 +6197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>1</v>
       </c>
@@ -6231,7 +6232,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>1</v>
       </c>
@@ -6269,7 +6270,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>9</v>
       </c>
@@ -6298,7 +6299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>9</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>1</v>
       </c>
@@ -6365,7 +6366,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>10</v>
       </c>
@@ -6394,7 +6395,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>2</v>
       </c>
@@ -6432,7 +6433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>11</v>
       </c>
@@ -6461,7 +6462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>11</v>
       </c>
@@ -6490,7 +6491,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>11</v>
       </c>
@@ -6519,7 +6520,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>11</v>
       </c>
@@ -6548,7 +6549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>11</v>
       </c>
@@ -6577,7 +6578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>3</v>
       </c>
@@ -6615,7 +6616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>12</v>
       </c>
@@ -6644,7 +6645,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>12</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>12</v>
       </c>
@@ -6699,7 +6700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>12</v>
       </c>
@@ -6728,7 +6729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>1</v>
       </c>
@@ -6766,7 +6767,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>1</v>
       </c>
@@ -6804,7 +6805,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>7</v>
       </c>
@@ -6856,7 +6857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>15</v>
       </c>
@@ -6885,7 +6886,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>15</v>
       </c>
@@ -6917,7 +6918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>15</v>
       </c>
@@ -6946,7 +6947,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>15</v>
       </c>
@@ -6975,7 +6976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>15</v>
       </c>
@@ -7004,7 +7005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>15</v>
       </c>
@@ -7033,7 +7034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B50">
         <v>15</v>
       </c>
@@ -7076,7 +7077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B51">
         <v>15</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B52">
         <v>15</v>
       </c>
@@ -7134,7 +7135,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>15</v>
       </c>
@@ -7163,7 +7164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B54">
         <v>15</v>
       </c>
@@ -7192,7 +7193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B55">
         <v>15</v>
       </c>
@@ -7221,7 +7222,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>15</v>
       </c>
@@ -7250,7 +7251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>15</v>
       </c>
@@ -7279,7 +7280,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>15</v>
       </c>
@@ -7308,7 +7309,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>15</v>
       </c>
@@ -7337,7 +7338,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14">
         <v>2</v>
       </c>
@@ -7378,7 +7379,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>16</v>
       </c>
@@ -7407,7 +7408,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>16</v>
       </c>
@@ -7436,7 +7437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>16</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>16</v>
       </c>
@@ -7494,7 +7495,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14">
         <v>1</v>
       </c>
@@ -7532,7 +7533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14">
         <v>1</v>
       </c>
@@ -7570,7 +7571,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B67">
         <f>WETL_ID!A23</f>
         <v>19</v>
@@ -7615,7 +7616,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B68">
         <f>WETL_ID!A24</f>
         <v>20</v>
@@ -7657,7 +7658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B69">
         <f>WETL_ID!A25</f>
         <v>21</v>
@@ -7699,7 +7700,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B70">
         <f>WETL_ID!A26</f>
         <v>22</v>
@@ -7741,7 +7742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B71">
         <f>WETL_ID!A27</f>
         <v>23</v>
@@ -7783,7 +7784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B72">
         <f>WETL_ID!A28</f>
         <v>24</v>
@@ -7828,7 +7829,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B73">
         <f>WETL_ID!A29</f>
         <v>25</v>
@@ -7873,7 +7874,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B74">
         <f>WETL_ID!A30</f>
         <v>26</v>
@@ -7911,7 +7912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B75">
         <f>WETL_ID!A31</f>
         <v>27</v>
@@ -7953,7 +7954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B76">
         <f>WETL_ID!A32</f>
         <v>28</v>
@@ -7995,7 +7996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B77">
         <f>WETL_ID!A33</f>
         <v>29</v>
@@ -8040,7 +8041,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B78">
         <f>WETL_ID!A34</f>
         <v>30</v>
@@ -8085,12 +8086,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>SUM(A1:A66)</f>
         <v>36</v>
@@ -8099,7 +8100,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E81">
         <v>8177</v>
       </c>
@@ -8125,7 +8126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E82">
         <v>8121</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E83">
         <v>8121</v>
       </c>
@@ -8181,7 +8182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E84">
         <v>8210</v>
       </c>
@@ -8209,7 +8210,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E85">
         <v>8210</v>
       </c>
@@ -8237,7 +8238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E86">
         <v>8048</v>
       </c>
@@ -8265,7 +8266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E87">
         <v>8048</v>
       </c>
@@ -8291,7 +8292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E88">
         <v>8048</v>
       </c>
@@ -8319,7 +8320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E89">
         <v>8032</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="90" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E90">
         <v>8032</v>
       </c>
@@ -8377,7 +8378,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E91">
         <v>8059</v>
       </c>
@@ -8406,7 +8407,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E92">
         <v>8059</v>
       </c>
@@ -8435,7 +8436,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E93">
         <v>8059</v>
       </c>
@@ -8464,7 +8465,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E94">
         <v>8059</v>
       </c>
@@ -8493,7 +8494,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="95" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:17" x14ac:dyDescent="0.25">
       <c r="L95" s="5" t="s">
         <v>20</v>
       </c>
@@ -8509,10 +8510,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:17" x14ac:dyDescent="0.25">
       <c r="N96"/>
     </row>
-    <row r="97" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L97" s="5" t="s">
         <v>20</v>
       </c>
@@ -8528,7 +8529,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L99" s="5" t="s">
         <v>20</v>
       </c>
@@ -8544,7 +8545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L101" s="5" t="s">
         <v>20</v>
       </c>
@@ -8560,7 +8561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L103" s="5" t="s">
         <v>20</v>
       </c>
@@ -8576,7 +8577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L105" s="5" t="s">
         <v>17</v>
       </c>
@@ -8592,7 +8593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L107" s="5" t="s">
         <v>20</v>
       </c>
@@ -8608,7 +8609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L109" s="5" t="s">
         <v>17</v>
       </c>
@@ -8624,7 +8625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L111" s="5" t="s">
         <v>20</v>
       </c>
@@ -8640,7 +8641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L113" s="5" t="s">
         <v>20</v>
       </c>
@@ -8656,7 +8657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L115" s="5" t="s">
         <v>20</v>
       </c>
@@ -8672,7 +8673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L117" s="5" t="s">
         <v>20</v>
       </c>
@@ -8688,7 +8689,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L119" s="5" t="s">
         <v>20</v>
       </c>
@@ -8704,7 +8705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L121" s="5" t="s">
         <v>20</v>
       </c>
@@ -8720,7 +8721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L123" s="5" t="s">
         <v>20</v>
       </c>
@@ -8736,7 +8737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L125" s="5" t="s">
         <v>20</v>
       </c>
@@ -8752,7 +8753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L127" s="5" t="s">
         <v>20</v>
       </c>
@@ -8768,11 +8769,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="12:15" x14ac:dyDescent="0.25">
       <c r="L128" s="5"/>
       <c r="M128" s="4"/>
     </row>
-    <row r="129" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L129" s="5" t="s">
         <v>20</v>
       </c>
@@ -8788,7 +8789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C130">
         <f>SUM(C29:C129)</f>
         <v>63</v>
@@ -8796,7 +8797,7 @@
       <c r="L130" s="5"/>
       <c r="M130" s="4"/>
     </row>
-    <row r="132" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L132" s="5" t="s">
         <v>20</v>
       </c>
@@ -8812,11 +8813,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L133" s="5"/>
       <c r="M133" s="4"/>
     </row>
-    <row r="134" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L134" s="5" t="s">
         <v>20</v>
       </c>
@@ -8832,11 +8833,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L135" s="5"/>
       <c r="M135" s="4"/>
     </row>
-    <row r="136" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L136" s="5" t="s">
         <v>20</v>
       </c>
@@ -8852,11 +8853,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L137" s="5"/>
       <c r="M137" s="4"/>
     </row>
-    <row r="138" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L138" s="5" t="s">
         <v>20</v>
       </c>
@@ -8872,11 +8873,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L139" s="5"/>
       <c r="M139" s="4"/>
     </row>
-    <row r="140" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L140" s="5" t="s">
         <v>20</v>
       </c>
@@ -8892,11 +8893,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L141" s="5"/>
       <c r="M141" s="4"/>
     </row>
-    <row r="142" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L142" s="5" t="s">
         <v>20</v>
       </c>
@@ -8912,7 +8913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:15" x14ac:dyDescent="0.25">
       <c r="L143" s="5"/>
       <c r="M143" s="4"/>
     </row>

</xml_diff>

<commit_message>
wr_pods_McKenzie.csv - Associate all the municipal water rights in the McKenzie basin with the Eugene-Springfield UGA, including the ones for the Marcola and Rainbow water districts, but except the ones for Blue River water district.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/Wetlands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CA89FC-C1FA-43AB-8729-35B52E90376D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E38E17-6D9C-43CE-B376-82FE7F0E43A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{BA8B6196-FC25-450E-B90E-DCCE11AF4D42}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="IDUs (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>